<commit_message>
Midpoint on Itau 400 returning development
</commit_message>
<xml_diff>
--- a/docs/Normalization.xlsx
+++ b/docs/Normalization.xlsx
@@ -3146,9 +3146,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3184,26 +3184,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3213,7 +3206,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3227,6 +3220,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -3234,16 +3234,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3258,37 +3273,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3310,7 +3303,22 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3325,18 +3333,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3379,127 +3379,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3517,7 +3403,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3529,37 +3529,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3583,6 +3583,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -3593,21 +3608,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3638,15 +3638,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3665,6 +3656,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -3675,138 +3675,138 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -8838,7 +8838,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -9671,7 +9671,7 @@
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="C22:C23"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
@@ -9679,13 +9679,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="1"/>
+  <sheetPr/>
   <dimension ref="A1:AMJ182"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9722,7 +9722,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="2" ht="13" customHeight="1" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -9733,7 +9733,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="3" ht="13" customHeight="1" spans="1:7">
       <c r="A3" s="6" t="s">
         <v>618</v>
       </c>
@@ -9756,7 +9756,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="4" ht="13" customHeight="1" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>620</v>
       </c>
@@ -9779,7 +9779,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="5" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="5" ht="13" customHeight="1" spans="1:7">
       <c r="A5" s="6" t="s">
         <v>624</v>
       </c>
@@ -9802,7 +9802,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="6" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="6" ht="13" customHeight="1" spans="1:7">
       <c r="A6" s="6" t="s">
         <v>628</v>
       </c>
@@ -9825,7 +9825,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="7" ht="13" customHeight="1" spans="1:7">
       <c r="A7" s="6" t="s">
         <v>631</v>
       </c>
@@ -9848,7 +9848,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="8" ht="13" customHeight="1" spans="1:7">
       <c r="A8" s="6" t="s">
         <v>49</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="9" ht="13" customHeight="1" spans="1:7">
       <c r="A9" s="6" t="s">
         <v>634</v>
       </c>
@@ -9884,7 +9884,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="10" ht="13" customHeight="1" spans="1:7">
       <c r="A10" s="6" t="s">
         <v>56</v>
       </c>
@@ -9901,7 +9901,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="11" ht="13" customHeight="1" spans="1:7">
       <c r="A11" s="6" t="s">
         <v>636</v>
       </c>
@@ -9916,7 +9916,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="12" ht="13" customHeight="1" spans="1:7">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>83</v>
@@ -9933,7 +9933,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="13" ht="13" customHeight="1" spans="1:7">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -9946,7 +9946,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="14" ht="13" customHeight="1" spans="1:7">
       <c r="A14" s="6" t="s">
         <v>303</v>
       </c>
@@ -9969,7 +9969,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="15" ht="13" customHeight="1" spans="1:7">
       <c r="A15" s="1" t="s">
         <v>639</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="16" ht="13" customHeight="1" spans="1:7">
       <c r="A16" s="6" t="s">
         <v>643</v>
       </c>
@@ -10015,7 +10015,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="17" ht="13" customHeight="1" spans="1:7">
       <c r="A17" s="6" t="s">
         <v>644</v>
       </c>
@@ -10038,7 +10038,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="18" ht="13" customHeight="1" spans="1:7">
       <c r="A18"/>
       <c r="B18" s="6" t="s">
         <v>647</v>
@@ -10055,7 +10055,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="19" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="19" ht="13" customHeight="1" spans="1:7">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -10068,7 +10068,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="20" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="20" ht="13" customHeight="1" spans="1:7">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -10081,7 +10081,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="21" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="21" ht="13" customHeight="1" spans="1:7">
       <c r="A21"/>
       <c r="B21" s="6" t="s">
         <v>653</v>
@@ -10094,7 +10094,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="22" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="22" ht="13" customHeight="1" spans="1:7">
       <c r="A22"/>
       <c r="B22" s="6" t="s">
         <v>655</v>
@@ -10122,7 +10122,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="24" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="24" ht="13" customHeight="1" spans="1:7">
       <c r="A24" s="6" t="s">
         <v>657</v>
       </c>
@@ -10137,7 +10137,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="25" ht="13" customHeight="1" spans="1:7">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -10150,7 +10150,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="26" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="26" ht="13" customHeight="1" spans="1:7">
       <c r="A26" s="6" t="s">
         <v>658</v>
       </c>
@@ -10171,7 +10171,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="27" ht="13" customHeight="1" spans="1:7">
       <c r="A27" s="6" t="s">
         <v>661</v>
       </c>
@@ -10194,7 +10194,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="28" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="28" ht="13" customHeight="1" spans="1:7">
       <c r="A28" s="4" t="s">
         <v>127</v>
       </c>
@@ -10205,7 +10205,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="29" ht="13" customHeight="1" spans="1:7">
       <c r="A29" s="6" t="s">
         <v>618</v>
       </c>
@@ -10228,7 +10228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="30" ht="13" customHeight="1" spans="1:7">
       <c r="A30" s="6"/>
       <c r="B30" s="7" t="s">
         <v>663</v>
@@ -10249,7 +10249,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="31" ht="13" customHeight="1" spans="1:7">
       <c r="A31" s="6"/>
       <c r="B31" s="6" t="s">
         <v>664</v>
@@ -10270,7 +10270,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="32" ht="13" customHeight="1" spans="1:7">
       <c r="A32" s="6" t="s">
         <v>49</v>
       </c>
@@ -10293,7 +10293,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="33" ht="13" customHeight="1" spans="1:7">
       <c r="A33" s="6" t="s">
         <v>634</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="34" ht="13" customHeight="1" spans="1:7">
       <c r="A34" s="6" t="s">
         <v>56</v>
       </c>
@@ -10329,7 +10329,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="35" ht="13" customHeight="1" spans="1:7">
       <c r="A35" s="6" t="s">
         <v>636</v>
       </c>
@@ -10346,7 +10346,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="36" ht="13" customHeight="1" spans="1:7">
       <c r="A36" s="6" t="s">
         <v>657</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="37" ht="13" customHeight="1" spans="1:7">
       <c r="A37" s="6" t="s">
         <v>665</v>
       </c>
@@ -10384,7 +10384,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="38" ht="13" customHeight="1" spans="1:7">
       <c r="A38" s="6" t="s">
         <v>667</v>
       </c>
@@ -10407,7 +10407,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="39" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="39" ht="13" customHeight="1" spans="1:8">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -10420,7 +10420,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="40" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="40" ht="13" customHeight="1" spans="1:8">
       <c r="A40" s="6" t="s">
         <v>174</v>
       </c>
@@ -10444,7 +10444,7 @@
       </c>
       <c r="H40"/>
     </row>
-    <row r="41" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="41" ht="13" customHeight="1" spans="1:8">
       <c r="A41" s="6" t="s">
         <v>672</v>
       </c>
@@ -10460,7 +10460,7 @@
       </c>
       <c r="H41"/>
     </row>
-    <row r="42" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="42" ht="13" customHeight="1" spans="1:8">
       <c r="A42" s="6"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -10474,7 +10474,7 @@
       </c>
       <c r="H42"/>
     </row>
-    <row r="43" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="43" ht="13" customHeight="1" spans="1:8">
       <c r="A43"/>
       <c r="B43" s="7" t="s">
         <v>673</v>
@@ -10492,7 +10492,7 @@
       </c>
       <c r="H43"/>
     </row>
-    <row r="44" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="44" ht="13" customHeight="1" spans="1:8">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -10505,7 +10505,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="45" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="45" ht="13" customHeight="1" spans="1:8">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -10519,7 +10519,7 @@
       </c>
       <c r="H45"/>
     </row>
-    <row r="46" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="46" ht="13" customHeight="1" spans="1:8">
       <c r="A46"/>
       <c r="B46" s="7" t="s">
         <v>169</v>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="H46"/>
     </row>
-    <row r="47" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="47" ht="13" customHeight="1" spans="1:8">
       <c r="A47"/>
       <c r="B47" s="7"/>
       <c r="C47"/>
@@ -10547,7 +10547,7 @@
       </c>
       <c r="H47"/>
     </row>
-    <row r="48" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="48" ht="13" customHeight="1" spans="1:8">
       <c r="A48" s="6" t="s">
         <v>679</v>
       </c>
@@ -10563,7 +10563,7 @@
       </c>
       <c r="H48"/>
     </row>
-    <row r="49" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="49" ht="13" customHeight="1" spans="1:8">
       <c r="A49" s="6" t="s">
         <v>680</v>
       </c>
@@ -10587,7 +10587,7 @@
       </c>
       <c r="H49"/>
     </row>
-    <row r="50" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="50" ht="13" customHeight="1" spans="1:8">
       <c r="A50" s="6" t="s">
         <v>684</v>
       </c>
@@ -10611,7 +10611,7 @@
       </c>
       <c r="H50"/>
     </row>
-    <row r="51" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="51" ht="13" customHeight="1" spans="1:8">
       <c r="A51"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
@@ -10625,7 +10625,7 @@
       </c>
       <c r="H51"/>
     </row>
-    <row r="52" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="52" ht="13" customHeight="1" spans="1:8">
       <c r="A52"/>
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
@@ -10639,7 +10639,7 @@
       </c>
       <c r="H52"/>
     </row>
-    <row r="53" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="53" ht="13" customHeight="1" spans="1:8">
       <c r="A53"/>
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
@@ -10652,7 +10652,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="54" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="54" ht="13" customHeight="1" spans="1:8">
       <c r="A54" s="6" t="s">
         <v>693</v>
       </c>
@@ -10668,7 +10668,7 @@
       </c>
       <c r="H54"/>
     </row>
-    <row r="55" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="55" ht="13" customHeight="1" spans="1:8">
       <c r="A55" s="6" t="s">
         <v>696</v>
       </c>
@@ -10684,7 +10684,7 @@
       </c>
       <c r="H55"/>
     </row>
-    <row r="56" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="56" ht="13" customHeight="1" spans="1:8">
       <c r="A56" s="6" t="s">
         <v>699</v>
       </c>
@@ -10698,7 +10698,7 @@
       </c>
       <c r="H56"/>
     </row>
-    <row r="57" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="57" ht="13" customHeight="1" spans="1:8">
       <c r="A57" s="6" t="s">
         <v>700</v>
       </c>
@@ -10712,7 +10712,7 @@
       </c>
       <c r="H57"/>
     </row>
-    <row r="58" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="58" ht="13" customHeight="1" spans="1:8">
       <c r="A58" s="6"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -10726,7 +10726,7 @@
       </c>
       <c r="H58"/>
     </row>
-    <row r="59" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="59" ht="13" customHeight="1" spans="1:8">
       <c r="A59" s="6"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -10740,7 +10740,7 @@
       </c>
       <c r="H59"/>
     </row>
-    <row r="60" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="60" ht="13" customHeight="1" spans="1:8">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -10754,7 +10754,7 @@
       </c>
       <c r="H60"/>
     </row>
-    <row r="61" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="61" ht="13" customHeight="1" spans="1:8">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -10768,7 +10768,7 @@
       </c>
       <c r="H61"/>
     </row>
-    <row r="62" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="62" ht="13" customHeight="1" spans="1:8">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="H62"/>
     </row>
-    <row r="63" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="63" ht="13" customHeight="1" spans="1:8">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -10796,7 +10796,7 @@
       </c>
       <c r="H63"/>
     </row>
-    <row r="64" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="64" ht="13" customHeight="1" spans="1:8">
       <c r="A64" s="6" t="s">
         <v>714</v>
       </c>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="H65"/>
     </row>
-    <row r="66" ht="13" hidden="1" customHeight="1" spans="1:8">
+    <row r="66" ht="13" customHeight="1" spans="1:8">
       <c r="A66" s="6"/>
       <c r="B66" s="7" t="s">
         <v>722</v>
@@ -10846,7 +10846,7 @@
       </c>
       <c r="H66"/>
     </row>
-    <row r="67" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="67" ht="13" customHeight="1" spans="1:1024">
       <c r="A67"/>
       <c r="B67" s="6"/>
       <c r="C67" s="6" t="s">
@@ -11876,7 +11876,7 @@
       <c r="AMI67"/>
       <c r="AMJ67"/>
     </row>
-    <row r="68" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="68" ht="13" customHeight="1" spans="1:1024">
       <c r="A68" s="6"/>
       <c r="B68" s="7" t="s">
         <v>724</v>
@@ -12906,7 +12906,7 @@
       <c r="AMI68"/>
       <c r="AMJ68"/>
     </row>
-    <row r="69" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="69" ht="13" customHeight="1" spans="1:1024">
       <c r="A69" s="6" t="s">
         <v>725</v>
       </c>
@@ -13946,7 +13946,7 @@
       <c r="AMI69"/>
       <c r="AMJ69"/>
     </row>
-    <row r="70" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="70" ht="13" customHeight="1" spans="1:1024">
       <c r="A70" s="6" t="s">
         <v>197</v>
       </c>
@@ -14986,7 +14986,7 @@
       <c r="AMI70"/>
       <c r="AMJ70"/>
     </row>
-    <row r="71" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="71" ht="13" customHeight="1" spans="1:1024">
       <c r="A71" s="6" t="s">
         <v>203</v>
       </c>
@@ -16026,7 +16026,7 @@
       <c r="AMI71"/>
       <c r="AMJ71"/>
     </row>
-    <row r="72" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="72" ht="13" customHeight="1" spans="1:1024">
       <c r="A72" s="6" t="s">
         <v>639</v>
       </c>
@@ -17066,7 +17066,7 @@
       <c r="AMI72"/>
       <c r="AMJ72"/>
     </row>
-    <row r="73" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="73" ht="13" customHeight="1" spans="1:1024">
       <c r="A73" s="6" t="s">
         <v>49</v>
       </c>
@@ -18106,7 +18106,7 @@
       <c r="AMI73"/>
       <c r="AMJ73"/>
     </row>
-    <row r="74" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="74" ht="13" customHeight="1" spans="1:1024">
       <c r="A74" s="6" t="s">
         <v>634</v>
       </c>
@@ -19140,7 +19140,7 @@
       <c r="AMI74"/>
       <c r="AMJ74"/>
     </row>
-    <row r="75" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="75" ht="13" customHeight="1" spans="1:1024">
       <c r="A75" s="6" t="s">
         <v>225</v>
       </c>
@@ -20180,7 +20180,7 @@
       <c r="AMI75"/>
       <c r="AMJ75"/>
     </row>
-    <row r="76" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="76" ht="13" customHeight="1" spans="1:1024">
       <c r="A76" s="6" t="s">
         <v>741</v>
       </c>
@@ -21220,7 +21220,7 @@
       <c r="AMI76"/>
       <c r="AMJ76"/>
     </row>
-    <row r="77" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="77" ht="13" customHeight="1" spans="1:1024">
       <c r="A77" s="6" t="s">
         <v>744</v>
       </c>
@@ -22260,7 +22260,7 @@
       <c r="AMI77"/>
       <c r="AMJ77"/>
     </row>
-    <row r="78" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="78" ht="13" customHeight="1" spans="1:1024">
       <c r="A78" s="6" t="s">
         <v>749</v>
       </c>
@@ -23296,7 +23296,7 @@
       <c r="AMI78"/>
       <c r="AMJ78"/>
     </row>
-    <row r="79" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="79" ht="13" customHeight="1" spans="1:1024">
       <c r="A79" s="6" t="s">
         <v>754</v>
       </c>
@@ -24336,7 +24336,7 @@
       <c r="AMI79"/>
       <c r="AMJ79"/>
     </row>
-    <row r="80" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="80" ht="13" customHeight="1" spans="1:1024">
       <c r="A80" s="6" t="s">
         <v>284</v>
       </c>
@@ -25376,7 +25376,7 @@
       <c r="AMI80"/>
       <c r="AMJ80"/>
     </row>
-    <row r="81" ht="13" hidden="1" customHeight="1" spans="1:1024">
+    <row r="81" ht="13" customHeight="1" spans="1:1024">
       <c r="A81" s="6" t="s">
         <v>270</v>
       </c>
@@ -26416,7 +26416,7 @@
       <c r="AMI81"/>
       <c r="AMJ81"/>
     </row>
-    <row r="82" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="82" ht="13" customHeight="1" spans="1:7">
       <c r="A82" s="6" t="s">
         <v>764</v>
       </c>
@@ -26431,7 +26431,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="83" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="83" ht="13" customHeight="1" spans="1:7">
       <c r="A83" s="6" t="s">
         <v>767</v>
       </c>
@@ -26454,7 +26454,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="84" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="84" ht="13" customHeight="1" spans="1:7">
       <c r="A84" s="6" t="s">
         <v>772</v>
       </c>
@@ -26477,7 +26477,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="85" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="85" ht="13" customHeight="1" spans="1:7">
       <c r="A85" s="6"/>
       <c r="B85" s="7" t="s">
         <v>777</v>
@@ -26494,7 +26494,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="86" ht="13" customHeight="1" spans="1:7">
       <c r="A86" s="6" t="s">
         <v>779</v>
       </c>
@@ -26515,7 +26515,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="87" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="87" ht="13" customHeight="1" spans="1:7">
       <c r="A87" s="6" t="s">
         <v>784</v>
       </c>
@@ -26530,7 +26530,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="88" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="88" ht="13" customHeight="1" spans="1:7">
       <c r="A88" s="6" t="s">
         <v>787</v>
       </c>
@@ -26545,7 +26545,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="89" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="89" ht="13" customHeight="1" spans="1:7">
       <c r="A89" s="6" t="s">
         <v>790</v>
       </c>
@@ -26560,7 +26560,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="90" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="90" ht="13" customHeight="1" spans="1:7">
       <c r="A90" s="6" t="s">
         <v>793</v>
       </c>
@@ -26577,7 +26577,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="91" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="91" ht="13" customHeight="1" spans="1:7">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="C91"/>
@@ -26590,7 +26590,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="92" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="92" ht="13" customHeight="1" spans="1:7">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -26603,7 +26603,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="93" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="93" ht="13" customHeight="1" spans="1:7">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -26618,7 +26618,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="94" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="94" ht="13" customHeight="1" spans="1:7">
       <c r="A94" s="6" t="s">
         <v>799</v>
       </c>
@@ -26633,7 +26633,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="95" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="95" ht="13" customHeight="1" spans="1:7">
       <c r="A95" s="6" t="s">
         <v>802</v>
       </c>
@@ -26646,7 +26646,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="96" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="96" ht="13" customHeight="1" spans="1:7">
       <c r="A96"/>
       <c r="B96" s="7" t="s">
         <v>804</v>
@@ -26659,7 +26659,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="97" ht="13" customHeight="1" spans="1:7">
       <c r="A97"/>
       <c r="B97" s="6" t="s">
         <v>805</v>
@@ -26672,7 +26672,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="98" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="98" ht="13" customHeight="1" spans="1:7">
       <c r="A98"/>
       <c r="B98" s="6" t="s">
         <v>807</v>
@@ -26685,7 +26685,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="99" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="99" ht="13" customHeight="1" spans="1:7">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99" s="6" t="s">
@@ -26698,7 +26698,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="100" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="100" ht="13" customHeight="1" spans="1:7">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100" s="6" t="s">
@@ -26711,7 +26711,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="101" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="101" ht="13" customHeight="1" spans="1:7">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101" s="6" t="s">
@@ -26724,7 +26724,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="102" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="102" ht="13" customHeight="1" spans="1:7">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102" s="6" t="s">
@@ -26737,7 +26737,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="103" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="103" ht="13" customHeight="1" spans="1:7">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103" s="6" t="s">
@@ -26750,7 +26750,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="104" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="104" ht="13" customHeight="1" spans="1:7">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104" s="6" t="s">
@@ -26763,7 +26763,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="105" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="105" ht="13" customHeight="1" spans="1:7">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105" s="6"/>
@@ -26776,7 +26776,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="106" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="106" ht="13" customHeight="1" spans="1:7">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106" s="6"/>
@@ -26789,7 +26789,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="107" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="107" ht="13" customHeight="1" spans="1:7">
       <c r="A107"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
@@ -26802,7 +26802,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="108" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="108" ht="13" customHeight="1" spans="1:7">
       <c r="A108" s="6"/>
       <c r="B108" s="6"/>
       <c r="C108"/>
@@ -26815,7 +26815,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="109" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="109" ht="13" customHeight="1" spans="1:7">
       <c r="A109" s="6"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
@@ -26828,7 +26828,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="110" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="110" ht="13" customHeight="1" spans="1:7">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
@@ -26841,7 +26841,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="111" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="111" ht="13" customHeight="1" spans="1:7">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="C111"/>
@@ -26854,7 +26854,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="112" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="112" ht="13" customHeight="1" spans="1:7">
       <c r="A112"/>
       <c r="B112" s="6"/>
       <c r="C112"/>
@@ -26867,7 +26867,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="113" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="113" ht="13" customHeight="1" spans="1:7">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
@@ -26880,7 +26880,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="114" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="114" ht="13" customHeight="1" spans="1:7">
       <c r="A114" s="6" t="s">
         <v>824</v>
       </c>
@@ -26899,7 +26899,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="115" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="115" ht="13" customHeight="1" spans="1:7">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
@@ -26912,7 +26912,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="116" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="116" ht="13" customHeight="1" spans="1:7">
       <c r="A116" s="6" t="s">
         <v>661</v>
       </c>
@@ -26935,7 +26935,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="117" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="117" ht="13" customHeight="1" spans="1:7">
       <c r="A117" s="4" t="s">
         <v>454</v>
       </c>
@@ -26946,7 +26946,7 @@
       <c r="F117" s="5"/>
       <c r="G117" s="5"/>
     </row>
-    <row r="118" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="118" ht="13" customHeight="1" spans="1:7">
       <c r="A118" s="6" t="s">
         <v>618</v>
       </c>
@@ -26969,7 +26969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="119" ht="13" customHeight="1" spans="1:7">
       <c r="A119" s="6" t="s">
         <v>830</v>
       </c>
@@ -26992,7 +26992,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="120" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="120" ht="13" customHeight="1" spans="1:7">
       <c r="A120" s="6" t="s">
         <v>834</v>
       </c>
@@ -27013,7 +27013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="121" ht="13" customHeight="1" spans="1:7">
       <c r="A121" s="6" t="s">
         <v>836</v>
       </c>
@@ -27036,7 +27036,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="122" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="122" ht="13" customHeight="1" spans="1:7">
       <c r="A122" s="6"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
@@ -27049,7 +27049,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="123" ht="13" customHeight="1" spans="1:7">
       <c r="A123"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -27062,7 +27062,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="124" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="124" ht="13" customHeight="1" spans="1:7">
       <c r="A124"/>
       <c r="B124"/>
       <c r="C124" s="6"/>
@@ -27075,7 +27075,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="125" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="125" ht="13" customHeight="1" spans="1:7">
       <c r="A125"/>
       <c r="B125"/>
       <c r="C125" s="6"/>
@@ -27088,7 +27088,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="126" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="126" ht="13" customHeight="1" spans="1:7">
       <c r="A126"/>
       <c r="B126"/>
       <c r="C126" s="6"/>
@@ -27101,7 +27101,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="127" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="127" ht="13" customHeight="1" spans="1:7">
       <c r="A127"/>
       <c r="B127"/>
       <c r="C127" s="6"/>
@@ -27114,7 +27114,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="128" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="128" ht="13" customHeight="1" spans="1:7">
       <c r="A128"/>
       <c r="B128"/>
       <c r="C128" s="6"/>
@@ -27127,7 +27127,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="129" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="129" ht="13" customHeight="1" spans="1:7">
       <c r="A129"/>
       <c r="B129"/>
       <c r="C129" s="6"/>
@@ -27140,7 +27140,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="130" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="130" ht="13" customHeight="1" spans="1:7">
       <c r="A130"/>
       <c r="B130" s="7" t="s">
         <v>847</v>
@@ -27157,7 +27157,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="131" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="131" ht="13" customHeight="1" spans="1:7">
       <c r="A131"/>
       <c r="B131" s="6" t="s">
         <v>849</v>
@@ -27172,7 +27172,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="132" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="132" ht="13" customHeight="1" spans="1:7">
       <c r="A132"/>
       <c r="B132" s="6" t="s">
         <v>850</v>
@@ -27185,7 +27185,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="133" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="133" ht="13" customHeight="1" spans="1:7">
       <c r="A133" s="6" t="s">
         <v>852</v>
       </c>
@@ -27202,7 +27202,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="134" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="134" ht="13" customHeight="1" spans="1:7">
       <c r="A134" s="6" t="s">
         <v>855</v>
       </c>
@@ -27219,7 +27219,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="135" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="135" ht="13" customHeight="1" spans="1:7">
       <c r="A135" s="6" t="s">
         <v>858</v>
       </c>
@@ -27236,7 +27236,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="136" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="136" ht="13" customHeight="1" spans="1:7">
       <c r="A136" s="6" t="s">
         <v>862</v>
       </c>
@@ -27251,7 +27251,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="137" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="137" ht="13" customHeight="1" spans="1:7">
       <c r="A137" s="6" t="s">
         <v>864</v>
       </c>
@@ -27266,7 +27266,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="138" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="138" ht="13" customHeight="1" spans="1:7">
       <c r="A138" s="6" t="s">
         <v>866</v>
       </c>
@@ -27281,7 +27281,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="139" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="139" ht="13" customHeight="1" spans="1:7">
       <c r="A139"/>
       <c r="B139"/>
       <c r="C139" s="6"/>
@@ -27294,7 +27294,7 @@
         <v>869</v>
       </c>
     </row>
-    <row r="140" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="140" ht="13" customHeight="1" spans="1:7">
       <c r="A140"/>
       <c r="B140"/>
       <c r="C140" s="6"/>
@@ -27307,7 +27307,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="141" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="141" ht="13" customHeight="1" spans="1:7">
       <c r="A141"/>
       <c r="B141"/>
       <c r="C141" s="6"/>
@@ -27320,7 +27320,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="142" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="142" ht="13" customHeight="1" spans="1:7">
       <c r="A142" s="6" t="s">
         <v>873</v>
       </c>
@@ -27335,7 +27335,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="143" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="143" ht="13" customHeight="1" spans="1:7">
       <c r="A143" s="6" t="s">
         <v>876</v>
       </c>
@@ -27350,7 +27350,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="144" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="144" ht="13" customHeight="1" spans="1:7">
       <c r="A144" s="6" t="s">
         <v>879</v>
       </c>
@@ -27365,7 +27365,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="145" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="145" ht="13" customHeight="1" spans="1:7">
       <c r="A145" s="6" t="s">
         <v>882</v>
       </c>
@@ -27380,7 +27380,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="146" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="146" ht="13" customHeight="1" spans="1:7">
       <c r="A146" s="6" t="s">
         <v>885</v>
       </c>
@@ -27395,7 +27395,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="147" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="147" ht="13" customHeight="1" spans="1:7">
       <c r="A147" s="6" t="s">
         <v>888</v>
       </c>
@@ -27410,7 +27410,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="148" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="148" ht="13" customHeight="1" spans="1:7">
       <c r="A148" s="6" t="s">
         <v>891</v>
       </c>
@@ -27423,7 +27423,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="149" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="149" ht="13" customHeight="1" spans="1:7">
       <c r="A149" s="6" t="s">
         <v>893</v>
       </c>
@@ -27436,7 +27436,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="150" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="150" ht="13" customHeight="1" spans="1:7">
       <c r="A150" s="6" t="s">
         <v>895</v>
       </c>
@@ -27449,7 +27449,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="151" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="151" ht="13" customHeight="1" spans="1:7">
       <c r="A151" s="6"/>
       <c r="B151" s="6" t="s">
         <v>897</v>
@@ -27462,7 +27462,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="152" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="152" ht="13" customHeight="1" spans="1:7">
       <c r="A152" s="6"/>
       <c r="B152" s="7" t="s">
         <v>899</v>
@@ -27475,7 +27475,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="153" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="153" ht="13" customHeight="1" spans="1:7">
       <c r="A153" s="6"/>
       <c r="B153" s="7" t="s">
         <v>901</v>
@@ -27488,7 +27488,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="154" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="154" ht="13" customHeight="1" spans="1:7">
       <c r="A154" s="6"/>
       <c r="B154" s="7" t="s">
         <v>903</v>
@@ -27501,7 +27501,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="155" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="155" ht="13" customHeight="1" spans="1:7">
       <c r="A155" s="6"/>
       <c r="B155" s="6" t="s">
         <v>905</v>
@@ -27514,7 +27514,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="156" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="156" ht="13" customHeight="1" spans="1:7">
       <c r="A156" s="6"/>
       <c r="B156" s="7" t="s">
         <v>907</v>
@@ -27527,7 +27527,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="157" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="157" ht="13" customHeight="1" spans="1:7">
       <c r="A157" s="6"/>
       <c r="B157" s="7" t="s">
         <v>909</v>
@@ -27540,7 +27540,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="158" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="158" ht="13" customHeight="1" spans="1:7">
       <c r="A158" s="6"/>
       <c r="B158" s="7" t="s">
         <v>911</v>
@@ -27553,7 +27553,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="159" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="159" ht="13" customHeight="1" spans="1:7">
       <c r="A159" s="6"/>
       <c r="B159" s="7" t="s">
         <v>913</v>
@@ -27566,7 +27566,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="160" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="160" ht="13" customHeight="1" spans="1:7">
       <c r="A160" s="6"/>
       <c r="B160" s="7" t="s">
         <v>915</v>
@@ -27579,7 +27579,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="161" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="161" ht="13" customHeight="1" spans="1:7">
       <c r="A161" s="6"/>
       <c r="B161" s="7" t="s">
         <v>917</v>
@@ -27592,7 +27592,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="162" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="162" ht="13" customHeight="1" spans="1:7">
       <c r="A162" s="6"/>
       <c r="B162" s="6" t="s">
         <v>919</v>
@@ -27605,7 +27605,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="163" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="163" ht="13" customHeight="1" spans="1:7">
       <c r="A163" s="6"/>
       <c r="B163" s="6" t="s">
         <v>921</v>
@@ -27618,7 +27618,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="164" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="164" ht="13" customHeight="1" spans="1:7">
       <c r="A164" s="6"/>
       <c r="B164" s="6" t="s">
         <v>923</v>
@@ -27631,7 +27631,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="165" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="165" ht="13" customHeight="1" spans="1:7">
       <c r="A165" s="6"/>
       <c r="B165" s="7" t="s">
         <v>925</v>
@@ -27644,7 +27644,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="166" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="166" ht="13" customHeight="1" spans="1:7">
       <c r="A166" s="6"/>
       <c r="B166" s="6" t="s">
         <v>927</v>
@@ -27657,7 +27657,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="167" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="167" ht="13" customHeight="1" spans="1:7">
       <c r="A167" s="6"/>
       <c r="B167" s="6" t="s">
         <v>929</v>
@@ -27670,7 +27670,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="168" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="168" ht="13" customHeight="1" spans="1:7">
       <c r="A168" s="6"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
@@ -27683,7 +27683,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="169" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="169" ht="13" customHeight="1" spans="1:7">
       <c r="A169" s="6"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
@@ -27698,7 +27698,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="170" ht="13" hidden="1" customHeight="1" spans="1:7">
+    <row r="170" ht="13" customHeight="1" spans="1:7">
       <c r="A170" s="6" t="s">
         <v>661</v>
       </c>
@@ -27818,15 +27818,8 @@
       <c r="F182" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G170">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="equal" val="message"/>
-        <customFilter operator="equal" val="motive"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511111111111111" footer="0.511111111111111"/>
+  <autoFilter ref="A1:G170"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
Adjusts on Itau returning schema according normalization
</commit_message>
<xml_diff>
--- a/docs/Normalization.xlsx
+++ b/docs/Normalization.xlsx
@@ -13,14 +13,14 @@
     <sheet name="CNAB 400 - Return" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'CNAB 400 - Return'!$A$1:$G$170</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'CNAB 400 - Return'!$A$1:$G$172</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938">
   <si>
     <t>Banco do Brasil</t>
   </si>
@@ -2298,7 +2298,13 @@
     <t>ourNumber2</t>
   </si>
   <si>
+    <t>generatedOurNumber</t>
+  </si>
+  <si>
     <t>ourNumber2Dac</t>
+  </si>
+  <si>
+    <t>generatedOurNumberDv</t>
   </si>
   <si>
     <t>ourNumberConference</t>
@@ -2778,7 +2784,13 @@
     <t>instCancel</t>
   </si>
   <si>
-    <t>canceledInstruction</t>
+    <t>otherMotive</t>
+  </si>
+  <si>
+    <t>payerClaimDate</t>
+  </si>
+  <si>
+    <t>payerClaimValue</t>
   </si>
   <si>
     <t>channel</t>
@@ -3145,10 +3157,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3184,68 +3196,11 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3256,72 +3211,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -3339,8 +3231,128 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3379,7 +3391,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.8"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3391,7 +3409,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3403,127 +3517,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3547,19 +3553,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3583,6 +3601,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -3598,16 +3631,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3619,21 +3652,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3656,8 +3674,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3665,8 +3683,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3675,142 +3693,142 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3839,6 +3857,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -8855,7 +8876,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47.2583333333333" style="10"/>
+    <col min="1" max="1" width="47.2583333333333" style="11"/>
     <col min="2" max="2" width="47.7416666666667"/>
     <col min="3" max="3" width="49.2583333333333"/>
   </cols>
@@ -8872,183 +8893,183 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>475</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>478</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" ht="146.25" spans="1:3">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" ht="97.5" spans="1:3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>487</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="13" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="12" t="s">
         <v>490</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="12" t="s">
         <v>491</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="12" t="s">
         <v>493</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>494</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="14" t="s">
         <v>495</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="15" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="12" t="s">
         <v>497</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="12" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="12" t="s">
         <v>499</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="14" t="s">
         <v>500</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="12" t="s">
         <v>502</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
     </row>
     <row r="24" ht="107.25" spans="1:3">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="12" t="s">
         <v>503</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="13" t="s">
         <v>505</v>
       </c>
     </row>
@@ -9064,90 +9085,90 @@
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="11" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="11" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="11" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="11" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="11" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="11" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="11" t="s">
         <v>520</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="11" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="11" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="11" t="s">
         <v>523</v>
       </c>
     </row>
@@ -9155,140 +9176,140 @@
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="16" t="s">
         <v>471</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="16" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="10" t="s">
+      <c r="A44" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11" t="s">
+      <c r="B44" s="12"/>
+      <c r="C44" s="12" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="45" ht="78" spans="1:3">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="11" t="s">
         <v>526</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="13" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="46" ht="29.25" spans="1:3">
-      <c r="A46" s="10" t="s">
+      <c r="A46" s="11" t="s">
         <v>529</v>
       </c>
-      <c r="B46" s="11" t="s">
+      <c r="B46" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="13" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="11" t="s">
         <v>532</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B47" s="12" t="s">
         <v>530</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="12" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="48" ht="19.5" spans="1:3">
-      <c r="A48" s="10" t="s">
+      <c r="A48" s="11" t="s">
         <v>534</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="12" t="s">
         <v>535</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="13" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="49" ht="19.5" spans="1:3">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="11" t="s">
         <v>537</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B49" s="12" t="s">
         <v>538</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="13" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="50" ht="29.25" spans="1:3">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>540</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="13" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="10" t="s">
+      <c r="A51" s="11" t="s">
         <v>543</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="12" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="52" ht="409.5" spans="1:3">
-      <c r="A52" s="10" t="s">
+      <c r="A52" s="11" t="s">
         <v>545</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="13" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="10" t="s">
+      <c r="A53" s="11" t="s">
         <v>547</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="12" t="s">
         <v>527</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="12" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="10" t="s">
+      <c r="A54" s="11" t="s">
         <v>549</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="12" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="10" t="s">
+      <c r="A55" s="11" t="s">
         <v>550</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="12" t="s">
         <v>541</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="12" t="s">
         <v>544</v>
       </c>
     </row>
@@ -9304,236 +9325,236 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="10" t="s">
+      <c r="A57" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="B57" s="11" t="s">
+      <c r="B57" s="12" t="s">
         <v>552</v>
       </c>
-      <c r="C57" s="11"/>
+      <c r="C57" s="12"/>
     </row>
     <row r="58" ht="87.75" spans="1:3">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="11" t="s">
         <v>553</v>
       </c>
-      <c r="B58" s="11"/>
-      <c r="C58" s="12" t="s">
+      <c r="B58" s="12"/>
+      <c r="C58" s="13" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="59" ht="107.25" spans="1:3">
-      <c r="A59" s="10" t="s">
+      <c r="A59" s="11" t="s">
         <v>555</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="13" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="11" t="s">
         <v>558</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="12" t="s">
         <v>556</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="11" t="s">
         <v>560</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="12" t="s">
         <v>561</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="11" t="s">
         <v>562</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="12" t="s">
         <v>563</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="11" t="s">
         <v>564</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="12" t="s">
         <v>565</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="64" ht="97.5" spans="1:3">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="12" t="s">
+      <c r="B64" s="12"/>
+      <c r="C64" s="13" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="11" t="s">
         <v>568</v>
       </c>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="11" t="s">
         <v>569</v>
       </c>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11" t="s">
+      <c r="B66" s="12"/>
+      <c r="C66" s="12" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="67" ht="48.75" spans="1:3">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="11" t="s">
         <v>570</v>
       </c>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12" t="s">
+      <c r="B67" s="12"/>
+      <c r="C67" s="13" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="68" ht="78" spans="1:3">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="11" t="s">
         <v>572</v>
       </c>
-      <c r="B68" s="11"/>
-      <c r="C68" s="12" t="s">
+      <c r="B68" s="12"/>
+      <c r="C68" s="13" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="11" t="s">
         <v>574</v>
       </c>
-      <c r="B69" s="11" t="s">
+      <c r="B69" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="C69" s="11" t="s">
+      <c r="C69" s="12" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="11" t="s">
         <v>577</v>
       </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11" t="s">
+      <c r="B70" s="12"/>
+      <c r="C70" s="12" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="71" ht="48.75" spans="1:3">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="11" t="s">
         <v>579</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="12" t="s">
         <v>580</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="13" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="11" t="s">
         <v>582</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="12" t="s">
         <v>561</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="C72" s="12" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="73" ht="39" spans="1:3">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="11" t="s">
         <v>583</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="12" t="s">
         <v>584</v>
       </c>
-      <c r="C73" s="12" t="s">
+      <c r="C73" s="13" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="11" t="s">
         <v>586</v>
       </c>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11" t="s">
+      <c r="B74" s="12"/>
+      <c r="C74" s="12" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="11" t="s">
         <v>587</v>
       </c>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11" t="s">
+      <c r="B75" s="12"/>
+      <c r="C75" s="12" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="76" ht="97.5" spans="1:3">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="11" t="s">
         <v>588</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="C76" s="12" t="s">
+      <c r="B76" s="12"/>
+      <c r="C76" s="13" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="11" t="s">
         <v>590</v>
       </c>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11" t="s">
+      <c r="B77" s="12"/>
+      <c r="C77" s="12" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="78" ht="48.75" spans="1:3">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="11" t="s">
         <v>591</v>
       </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="12" t="s">
+      <c r="B78" s="12"/>
+      <c r="C78" s="13" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="79" ht="107.25" spans="1:3">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="11" t="s">
         <v>593</v>
       </c>
-      <c r="B79" s="11"/>
-      <c r="C79" s="12" t="s">
+      <c r="B79" s="12"/>
+      <c r="C79" s="13" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="80" ht="39" spans="1:3">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="11" t="s">
         <v>595</v>
       </c>
-      <c r="B80" s="11"/>
-      <c r="C80" s="12" t="s">
+      <c r="B80" s="12"/>
+      <c r="C80" s="13" t="s">
         <v>596</v>
       </c>
     </row>
@@ -9549,62 +9570,62 @@
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="11" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="11" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="10" t="s">
+      <c r="A84" s="11" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="11" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="10" t="s">
+      <c r="A86" s="11" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="10" t="s">
+      <c r="A87" s="11" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="10" t="s">
+      <c r="A88" s="11" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="10" t="s">
+      <c r="A89" s="11" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="10" t="s">
+      <c r="A90" s="11" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="10" t="s">
+      <c r="A91" s="11" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="10" t="s">
+      <c r="A92" s="11" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="10" t="s">
+      <c r="A93" s="11" t="s">
         <v>608</v>
       </c>
     </row>
@@ -9620,47 +9641,47 @@
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="10" t="s">
+      <c r="A95" s="11" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="10" t="s">
+      <c r="A96" s="11" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="10" t="s">
+      <c r="A97" s="11" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="10" t="s">
+      <c r="A98" s="11" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="10" t="s">
+      <c r="A99" s="11" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="10" t="s">
+      <c r="A100" s="11" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="10" t="s">
+      <c r="A101" s="11" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="10" t="s">
+      <c r="A102" s="11" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="10" t="s">
+      <c r="A103" s="11" t="s">
         <v>617</v>
       </c>
     </row>
@@ -9680,12 +9701,12 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AMJ182"/>
+  <dimension ref="A1:AMJ184"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -10488,21 +10509,21 @@
         <v>166</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="H43"/>
     </row>
-    <row r="44" ht="13" customHeight="1" spans="1:8">
+    <row r="44" ht="13" customHeight="1" spans="1:7">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
       <c r="D44" s="6" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E44"/>
       <c r="F44"/>
-      <c r="H44" s="1" t="s">
-        <v>671</v>
+      <c r="G44" s="2" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="45" ht="13" customHeight="1" spans="1:8">
@@ -10510,12 +10531,12 @@
       <c r="B45"/>
       <c r="C45"/>
       <c r="D45" s="6" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="E45"/>
       <c r="F45"/>
       <c r="G45" s="2" t="s">
-        <v>676</v>
+        <v>678</v>
       </c>
       <c r="H45"/>
     </row>
@@ -10529,7 +10550,7 @@
       <c r="E46"/>
       <c r="F46"/>
       <c r="G46" s="2" t="s">
-        <v>677</v>
+        <v>679</v>
       </c>
       <c r="H46"/>
     </row>
@@ -10539,7 +10560,7 @@
       <c r="C47"/>
       <c r="D47" s="6"/>
       <c r="E47" s="7" t="s">
-        <v>678</v>
+        <v>680</v>
       </c>
       <c r="F47"/>
       <c r="G47" s="2" t="s">
@@ -10549,7 +10570,7 @@
     </row>
     <row r="48" ht="13" customHeight="1" spans="1:8">
       <c r="A48" s="6" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="B48"/>
       <c r="C48"/>
@@ -10565,10 +10586,10 @@
     </row>
     <row r="49" ht="13" customHeight="1" spans="1:8">
       <c r="A49" s="6" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>681</v>
+        <v>683</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>189</v>
@@ -10577,10 +10598,10 @@
         <v>189</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>189</v>
@@ -10589,25 +10610,25 @@
     </row>
     <row r="50" ht="13" customHeight="1" spans="1:8">
       <c r="A50" s="6" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="F50" s="6" t="s">
+        <v>690</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>688</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>686</v>
       </c>
       <c r="H50"/>
     </row>
@@ -10617,7 +10638,7 @@
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="F51"/>
       <c r="G51" s="2" t="s">
@@ -10632,7 +10653,7 @@
       <c r="D52" s="6"/>
       <c r="E52"/>
       <c r="F52" s="6" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>151</v>
@@ -10645,48 +10666,48 @@
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="F53"/>
       <c r="H53" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
     </row>
     <row r="54" ht="13" customHeight="1" spans="1:8">
       <c r="A54" s="6" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="F54"/>
       <c r="G54" s="2" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="H54"/>
     </row>
     <row r="55" ht="13" customHeight="1" spans="1:8">
       <c r="A55" s="6" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="B55"/>
       <c r="C55"/>
       <c r="D55"/>
       <c r="E55" s="6" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="F55"/>
       <c r="G55" s="2" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="H55"/>
     </row>
     <row r="56" ht="13" customHeight="1" spans="1:8">
       <c r="A56" s="6" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="B56"/>
       <c r="C56"/>
@@ -10700,7 +10721,7 @@
     </row>
     <row r="57" ht="13" customHeight="1" spans="1:8">
       <c r="A57" s="6" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B57"/>
       <c r="C57"/>
@@ -10708,7 +10729,7 @@
       <c r="E57" s="6"/>
       <c r="F57"/>
       <c r="G57" s="2" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="H57"/>
     </row>
@@ -10719,10 +10740,10 @@
       <c r="D58"/>
       <c r="E58" s="6"/>
       <c r="F58" s="6" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="H58"/>
     </row>
@@ -10733,10 +10754,10 @@
       <c r="D59"/>
       <c r="E59" s="6"/>
       <c r="F59" s="6" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="H59"/>
     </row>
@@ -10747,10 +10768,10 @@
       <c r="D60"/>
       <c r="E60"/>
       <c r="F60" s="6" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="H60"/>
     </row>
@@ -10761,10 +10782,10 @@
       <c r="D61"/>
       <c r="E61"/>
       <c r="F61" s="6" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="H61"/>
     </row>
@@ -10774,11 +10795,11 @@
       <c r="C62"/>
       <c r="D62"/>
       <c r="E62" s="6" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="F62" s="6"/>
       <c r="G62" s="2" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="H62"/>
     </row>
@@ -10788,17 +10809,17 @@
       <c r="C63"/>
       <c r="D63"/>
       <c r="E63" s="6" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="F63" s="6"/>
       <c r="G63" s="2" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="H63"/>
     </row>
     <row r="64" ht="13" customHeight="1" spans="1:8">
       <c r="A64" s="6" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="B64"/>
       <c r="C64"/>
@@ -10806,43 +10827,43 @@
       <c r="E64" s="6"/>
       <c r="F64"/>
       <c r="G64" s="2" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="H64"/>
     </row>
     <row r="65" ht="13" customHeight="1" spans="1:8">
       <c r="A65" s="6" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="F65"/>
       <c r="G65" s="9" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="H65"/>
     </row>
     <row r="66" ht="13" customHeight="1" spans="1:8">
       <c r="A66" s="6"/>
       <c r="B66" s="7" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="C66"/>
       <c r="D66"/>
       <c r="E66" s="6"/>
       <c r="F66"/>
       <c r="G66" s="9" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="H66"/>
     </row>
@@ -11879,7 +11900,7 @@
     <row r="68" ht="13" customHeight="1" spans="1:1024">
       <c r="A68" s="6"/>
       <c r="B68" s="7" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="C68"/>
       <c r="D68"/>
@@ -12908,16 +12929,16 @@
     </row>
     <row r="69" ht="13" customHeight="1" spans="1:1024">
       <c r="A69" s="6" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>360</v>
@@ -13951,16 +13972,16 @@
         <v>197</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D70" s="6" t="s">
+      <c r="D70" s="10" t="s">
         <v>197</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>196</v>
@@ -15000,10 +15021,10 @@
         <v>203</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>203</v>
@@ -16031,7 +16052,7 @@
         <v>639</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>210</v>
@@ -16040,10 +16061,10 @@
         <v>210</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>210</v>
@@ -17071,7 +17092,7 @@
         <v>49</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>216</v>
@@ -17080,10 +17101,10 @@
         <v>216</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>216</v>
@@ -18113,10 +18134,10 @@
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74" s="6" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="F74"/>
       <c r="G74" s="2" t="s">
@@ -19145,7 +19166,7 @@
         <v>225</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>225</v>
@@ -20182,7 +20203,7 @@
     </row>
     <row r="76" ht="13" customHeight="1" spans="1:1024">
       <c r="A76" s="6" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>655</v>
@@ -20194,10 +20215,10 @@
         <v>656</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>656</v>
@@ -21222,25 +21243,25 @@
     </row>
     <row r="77" ht="13" customHeight="1" spans="1:1024">
       <c r="A77" s="6" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="F77" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>748</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>746</v>
       </c>
       <c r="H77"/>
       <c r="I77"/>
@@ -22262,21 +22283,21 @@
     </row>
     <row r="78" ht="13" customHeight="1" spans="1:1024">
       <c r="A78" s="6" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78" s="6" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="H78"/>
       <c r="I78"/>
@@ -23298,10 +23319,10 @@
     </row>
     <row r="79" ht="13" customHeight="1" spans="1:1024">
       <c r="A79" s="6" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>277</v>
@@ -23310,10 +23331,10 @@
         <v>277</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>277</v>
@@ -24341,7 +24362,7 @@
         <v>284</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>284</v>
@@ -24350,10 +24371,10 @@
         <v>284</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>284</v>
@@ -25381,7 +25402,7 @@
         <v>270</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>270</v>
@@ -25390,10 +25411,10 @@
         <v>270</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>270</v>
@@ -26418,69 +26439,69 @@
     </row>
     <row r="82" ht="13" customHeight="1" spans="1:7">
       <c r="A82" s="6" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82" s="6" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="F82"/>
       <c r="G82" s="2" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
     </row>
     <row r="83" ht="13" customHeight="1" spans="1:7">
       <c r="A83" s="6" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="F83" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>771</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="84" ht="13" customHeight="1" spans="1:7">
       <c r="A84" s="6" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="D84" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>775</v>
       </c>
-      <c r="E84" s="6" t="s">
-        <v>773</v>
-      </c>
       <c r="F84" s="6" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
     </row>
     <row r="85" ht="13" customHeight="1" spans="1:7">
       <c r="A85" s="6"/>
       <c r="B85" s="7" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>439</v>
@@ -26488,7 +26509,7 @@
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>439</v>
@@ -26496,85 +26517,85 @@
     </row>
     <row r="86" ht="13" customHeight="1" spans="1:7">
       <c r="A86" s="6" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C86"/>
       <c r="D86" s="6" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="F86" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>783</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="87" ht="13" customHeight="1" spans="1:7">
       <c r="A87" s="6" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="2" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
     </row>
     <row r="88" ht="13" customHeight="1" spans="1:7">
       <c r="A88" s="6" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="2" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
     </row>
     <row r="89" ht="13" customHeight="1" spans="1:7">
       <c r="A89" s="6" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="2" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
     </row>
     <row r="90" ht="13" customHeight="1" spans="1:7">
       <c r="A90" s="6" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
     </row>
     <row r="91" ht="13" customHeight="1" spans="1:7">
@@ -26584,10 +26605,10 @@
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="F91" s="6" t="s">
+        <v>799</v>
+      </c>
+      <c r="G91" s="2" t="s">
         <v>797</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="92" ht="13" customHeight="1" spans="1:7">
@@ -26597,7 +26618,7 @@
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92" s="6" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>231</v>
@@ -26620,22 +26641,22 @@
     </row>
     <row r="94" ht="13" customHeight="1" spans="1:7">
       <c r="A94" s="6" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94" s="6" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="2" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
     <row r="95" ht="13" customHeight="1" spans="1:7">
       <c r="A95" s="6" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="B95"/>
       <c r="C95"/>
@@ -26643,13 +26664,13 @@
       <c r="E95"/>
       <c r="F95" s="6"/>
       <c r="G95" s="2" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
     <row r="96" ht="13" customHeight="1" spans="1:7">
       <c r="A96"/>
       <c r="B96" s="7" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C96"/>
       <c r="D96"/>
@@ -26662,92 +26683,92 @@
     <row r="97" ht="13" customHeight="1" spans="1:7">
       <c r="A97"/>
       <c r="B97" s="6" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
       <c r="F97" s="6"/>
       <c r="G97" s="2" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
     <row r="98" ht="13" customHeight="1" spans="1:7">
       <c r="A98"/>
       <c r="B98" s="6" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
       <c r="F98" s="6"/>
       <c r="G98" s="2" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
     <row r="99" ht="13" customHeight="1" spans="1:7">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99" s="6" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99" s="6"/>
       <c r="G99" s="2" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
     <row r="100" ht="13" customHeight="1" spans="1:7">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100" s="6" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D100"/>
       <c r="E100"/>
       <c r="F100"/>
       <c r="G100" s="2" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
     </row>
     <row r="101" ht="13" customHeight="1" spans="1:7">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101" s="6" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
       <c r="G101" s="2" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="102" ht="13" customHeight="1" spans="1:7">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102" s="6" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
       <c r="G102" s="2" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
     </row>
     <row r="103" ht="13" customHeight="1" spans="1:7">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103" s="6" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
       <c r="G103" s="2" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:7">
@@ -26769,7 +26790,7 @@
       <c r="C105" s="6"/>
       <c r="D105"/>
       <c r="E105" s="6" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="2" t="s">
@@ -26783,10 +26804,10 @@
       <c r="D106" s="6"/>
       <c r="E106"/>
       <c r="F106" s="6" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="107" ht="13" customHeight="1" spans="1:7">
@@ -26796,10 +26817,10 @@
       <c r="D107" s="6"/>
       <c r="E107"/>
       <c r="F107" s="6" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
     </row>
     <row r="108" ht="13" customHeight="1" spans="1:7">
@@ -26851,7 +26872,7 @@
         <v>415</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
     </row>
     <row r="112" ht="13" customHeight="1" spans="1:7">
@@ -26859,12 +26880,12 @@
       <c r="B112" s="6"/>
       <c r="C112"/>
       <c r="D112" s="6" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="E112" s="6"/>
       <c r="F112"/>
       <c r="G112" s="2" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="113" ht="13" customHeight="1" spans="1:7">
@@ -26872,220 +26893,220 @@
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="E113" s="6"/>
       <c r="F113" s="6"/>
       <c r="G113" s="2" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:7">
-      <c r="A114" s="6" t="s">
-        <v>824</v>
-      </c>
-      <c r="B114" s="6" t="s">
-        <v>825</v>
-      </c>
-      <c r="C114" s="6" t="s">
-        <v>824</v>
-      </c>
+      <c r="A114" s="6"/>
+      <c r="B114" s="6"/>
+      <c r="C114" s="6"/>
       <c r="D114" s="6" t="s">
         <v>826</v>
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="6"/>
       <c r="G114" s="2" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
     </row>
     <row r="115" ht="13" customHeight="1" spans="1:7">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
+      <c r="D115" s="6" t="s">
+        <v>827</v>
+      </c>
       <c r="E115" s="6"/>
-      <c r="F115" s="6" t="s">
-        <v>660</v>
-      </c>
+      <c r="F115" s="6"/>
       <c r="G115" s="2" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="116" ht="13" customHeight="1" spans="1:7">
       <c r="A116" s="6" t="s">
-        <v>661</v>
-      </c>
-      <c r="B116" s="7" t="s">
         <v>828</v>
       </c>
+      <c r="B116" s="6" t="s">
+        <v>829</v>
+      </c>
       <c r="C116" s="6" t="s">
-        <v>126</v>
+        <v>828</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="F116" s="6" t="s">
-        <v>125</v>
-      </c>
+        <v>830</v>
+      </c>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
       <c r="G116" s="2" t="s">
-        <v>126</v>
+        <v>828</v>
       </c>
     </row>
     <row r="117" ht="13" customHeight="1" spans="1:7">
-      <c r="A117" s="4" t="s">
-        <v>454</v>
-      </c>
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
+      <c r="A117" s="6"/>
+      <c r="B117" s="6"/>
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:7">
       <c r="A118" s="6" t="s">
-        <v>618</v>
+        <v>661</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>12</v>
+        <v>832</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>829</v>
+        <v>470</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>17</v>
+        <v>126</v>
       </c>
     </row>
     <row r="119" ht="13" customHeight="1" spans="1:7">
-      <c r="A119" s="6" t="s">
-        <v>830</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>831</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>622</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>622</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>832</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>833</v>
-      </c>
-      <c r="G119" s="2" t="s">
-        <v>622</v>
-      </c>
+      <c r="A119" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B119" s="5"/>
+      <c r="C119" s="5"/>
+      <c r="D119" s="5"/>
+      <c r="E119" s="5"/>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
     </row>
     <row r="120" ht="13" customHeight="1" spans="1:7">
       <c r="A120" s="6" t="s">
-        <v>834</v>
+        <v>618</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>835</v>
+        <v>12</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E120"/>
+        <v>17</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>833</v>
+      </c>
       <c r="F120" s="6" t="s">
-        <v>630</v>
+        <v>16</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
     </row>
     <row r="121" ht="13" customHeight="1" spans="1:7">
       <c r="A121" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="E121" s="6" t="s">
         <v>836</v>
       </c>
-      <c r="B121" s="6" t="s">
+      <c r="F121" s="6" t="s">
+        <v>837</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="122" ht="13" customHeight="1" spans="1:7">
+      <c r="A122" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E122"/>
+      <c r="F122" s="6" t="s">
+        <v>630</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="123" ht="13" customHeight="1" spans="1:7">
+      <c r="A123" s="6" t="s">
+        <v>840</v>
+      </c>
+      <c r="B123" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C121" s="6" t="s">
+      <c r="C123" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D121" s="6" t="s">
+      <c r="D123" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E121" s="6" t="s">
+      <c r="E123" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F121" s="6" t="s">
+      <c r="F123" s="6" t="s">
         <v>642</v>
       </c>
-      <c r="G121" s="2" t="s">
+      <c r="G123" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="122" ht="13" customHeight="1" spans="1:7">
-      <c r="A122" s="6"/>
-      <c r="B122" s="6"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="6" t="s">
-        <v>837</v>
-      </c>
-      <c r="F122" s="6"/>
-      <c r="G122" s="2" t="s">
+    <row r="124" ht="13" customHeight="1" spans="1:7">
+      <c r="A124" s="6"/>
+      <c r="B124" s="6"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="6"/>
+      <c r="E124" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="F124" s="6"/>
+      <c r="G124" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="123" ht="13" customHeight="1" spans="1:7">
-      <c r="A123"/>
-      <c r="B123"/>
-      <c r="C123"/>
-      <c r="D123"/>
-      <c r="E123" s="6" t="s">
-        <v>838</v>
-      </c>
-      <c r="F123"/>
-      <c r="G123" s="2" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="124" ht="13" customHeight="1" spans="1:7">
-      <c r="A124"/>
-      <c r="B124"/>
-      <c r="C124" s="6"/>
-      <c r="D124"/>
-      <c r="E124" s="6" t="s">
-        <v>840</v>
-      </c>
-      <c r="F124"/>
-      <c r="G124" s="2" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="125" ht="13" customHeight="1" spans="1:7">
       <c r="A125"/>
       <c r="B125"/>
-      <c r="C125" s="6"/>
+      <c r="C125"/>
       <c r="D125"/>
       <c r="E125" s="6" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F125"/>
       <c r="G125" s="2" t="s">
-        <v>315</v>
+        <v>843</v>
       </c>
     </row>
     <row r="126" ht="13" customHeight="1" spans="1:7">
@@ -27094,11 +27115,11 @@
       <c r="C126" s="6"/>
       <c r="D126"/>
       <c r="E126" s="6" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="F126"/>
       <c r="G126" s="2" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
     </row>
     <row r="127" ht="13" customHeight="1" spans="1:7">
@@ -27107,11 +27128,11 @@
       <c r="C127" s="6"/>
       <c r="D127"/>
       <c r="E127" s="6" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F127"/>
       <c r="G127" s="2" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" ht="13" customHeight="1" spans="1:7">
@@ -27120,11 +27141,11 @@
       <c r="C128" s="6"/>
       <c r="D128"/>
       <c r="E128" s="6" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="F128"/>
       <c r="G128" s="2" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="129" ht="13" customHeight="1" spans="1:7">
@@ -27133,135 +27154,131 @@
       <c r="C129" s="6"/>
       <c r="D129"/>
       <c r="E129" s="6" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="F129"/>
       <c r="G129" s="2" t="s">
-        <v>846</v>
+        <v>327</v>
       </c>
     </row>
     <row r="130" ht="13" customHeight="1" spans="1:7">
       <c r="A130"/>
-      <c r="B130" s="7" t="s">
-        <v>847</v>
-      </c>
+      <c r="B130"/>
       <c r="C130" s="6"/>
-      <c r="D130" s="6" t="s">
-        <v>459</v>
-      </c>
+      <c r="D130"/>
       <c r="E130" s="6" t="s">
         <v>848</v>
       </c>
       <c r="F130"/>
       <c r="G130" s="2" t="s">
-        <v>459</v>
+        <v>333</v>
       </c>
     </row>
     <row r="131" ht="13" customHeight="1" spans="1:7">
       <c r="A131"/>
-      <c r="B131" s="6" t="s">
+      <c r="B131"/>
+      <c r="C131" s="6"/>
+      <c r="D131"/>
+      <c r="E131" s="6" t="s">
         <v>849</v>
       </c>
-      <c r="C131" s="6"/>
-      <c r="D131" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="E131" s="6"/>
       <c r="F131"/>
       <c r="G131" s="2" t="s">
-        <v>203</v>
+        <v>850</v>
       </c>
     </row>
     <row r="132" ht="13" customHeight="1" spans="1:7">
       <c r="A132"/>
-      <c r="B132" s="6" t="s">
-        <v>850</v>
+      <c r="B132" s="7" t="s">
+        <v>851</v>
       </c>
       <c r="C132" s="6"/>
-      <c r="D132" s="6"/>
-      <c r="E132" s="6"/>
+      <c r="D132" s="6" t="s">
+        <v>459</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>852</v>
+      </c>
       <c r="F132"/>
       <c r="G132" s="2" t="s">
-        <v>851</v>
+        <v>459</v>
       </c>
     </row>
     <row r="133" ht="13" customHeight="1" spans="1:7">
-      <c r="A133" s="6" t="s">
-        <v>852</v>
-      </c>
-      <c r="B133"/>
+      <c r="A133"/>
+      <c r="B133" s="6" t="s">
+        <v>853</v>
+      </c>
       <c r="C133" s="6"/>
       <c r="D133" s="6" t="s">
-        <v>853</v>
-      </c>
-      <c r="E133"/>
-      <c r="F133" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E133" s="6"/>
+      <c r="F133"/>
+      <c r="G133" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="134" ht="13" customHeight="1" spans="1:7">
+      <c r="A134"/>
+      <c r="B134" s="6" t="s">
         <v>854</v>
       </c>
-      <c r="G133" s="2" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="134" ht="13" customHeight="1" spans="1:7">
-      <c r="A134" s="6" t="s">
+      <c r="C134" s="6"/>
+      <c r="D134" s="6"/>
+      <c r="E134" s="6"/>
+      <c r="F134"/>
+      <c r="G134" s="2" t="s">
         <v>855</v>
-      </c>
-      <c r="B134"/>
-      <c r="C134" s="6"/>
-      <c r="D134" s="6" t="s">
-        <v>856</v>
-      </c>
-      <c r="E134"/>
-      <c r="F134" s="6" t="s">
-        <v>857</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="135" ht="13" customHeight="1" spans="1:7">
       <c r="A135" s="6" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="B135"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6" t="s">
-        <v>859</v>
-      </c>
-      <c r="E135" s="6"/>
+        <v>857</v>
+      </c>
+      <c r="E135"/>
       <c r="F135" s="6" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="G135" s="2" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
     </row>
     <row r="136" ht="13" customHeight="1" spans="1:7">
       <c r="A136" s="6" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="B136"/>
       <c r="C136" s="6"/>
       <c r="D136" s="6" t="s">
-        <v>863</v>
-      </c>
-      <c r="E136" s="6"/>
-      <c r="F136"/>
+        <v>860</v>
+      </c>
+      <c r="E136"/>
+      <c r="F136" s="6" t="s">
+        <v>861</v>
+      </c>
       <c r="G136" s="2" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="137" ht="13" customHeight="1" spans="1:7">
       <c r="A137" s="6" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B137"/>
       <c r="C137" s="6"/>
       <c r="D137" s="6" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="E137" s="6"/>
-      <c r="F137"/>
+      <c r="F137" s="6" t="s">
+        <v>864</v>
+      </c>
       <c r="G137" s="2" t="s">
         <v>865</v>
       </c>
@@ -27278,11 +27295,13 @@
       <c r="E138" s="6"/>
       <c r="F138"/>
       <c r="G138" s="2" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="139" ht="13" customHeight="1" spans="1:7">
+      <c r="A139" s="6" t="s">
         <v>868</v>
       </c>
-    </row>
-    <row r="139" ht="13" customHeight="1" spans="1:7">
-      <c r="A139"/>
       <c r="B139"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6" t="s">
@@ -27295,16 +27314,18 @@
       </c>
     </row>
     <row r="140" ht="13" customHeight="1" spans="1:7">
-      <c r="A140"/>
+      <c r="A140" s="6" t="s">
+        <v>870</v>
+      </c>
       <c r="B140"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="E140" s="6"/>
       <c r="F140"/>
       <c r="G140" s="2" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
     </row>
     <row r="141" ht="13" customHeight="1" spans="1:7">
@@ -27312,126 +27333,126 @@
       <c r="B141"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="E141" s="6"/>
       <c r="F141"/>
       <c r="G141" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="142" ht="13" customHeight="1" spans="1:7">
-      <c r="A142" s="6" t="s">
-        <v>873</v>
-      </c>
+      <c r="A142"/>
       <c r="B142"/>
       <c r="C142" s="6"/>
-      <c r="D142"/>
+      <c r="D142" s="6" t="s">
+        <v>874</v>
+      </c>
       <c r="E142" s="6"/>
-      <c r="F142" s="6" t="s">
+      <c r="F142"/>
+      <c r="G142" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="G142" s="2" t="s">
-        <v>875</v>
-      </c>
     </row>
     <row r="143" ht="13" customHeight="1" spans="1:7">
-      <c r="A143" s="6" t="s">
-        <v>876</v>
-      </c>
+      <c r="A143"/>
       <c r="B143"/>
       <c r="C143" s="6"/>
-      <c r="D143"/>
+      <c r="D143" s="6" t="s">
+        <v>875</v>
+      </c>
       <c r="E143" s="6"/>
-      <c r="F143" s="6" t="s">
-        <v>877</v>
-      </c>
+      <c r="F143"/>
       <c r="G143" s="2" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="144" ht="13" customHeight="1" spans="1:7">
       <c r="A144" s="6" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="B144"/>
       <c r="C144" s="6"/>
       <c r="D144"/>
       <c r="E144" s="6"/>
       <c r="F144" s="6" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="145" ht="13" customHeight="1" spans="1:7">
       <c r="A145" s="6" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B145"/>
       <c r="C145" s="6"/>
-      <c r="D145" s="6"/>
+      <c r="D145"/>
       <c r="E145" s="6"/>
       <c r="F145" s="6" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="146" ht="13" customHeight="1" spans="1:7">
       <c r="A146" s="6" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="B146"/>
       <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
+      <c r="D146"/>
       <c r="E146" s="6"/>
       <c r="F146" s="6" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="147" ht="13" customHeight="1" spans="1:7">
       <c r="A147" s="6" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="B147"/>
       <c r="C147" s="6"/>
       <c r="D147" s="6"/>
       <c r="E147" s="6"/>
       <c r="F147" s="6" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
     </row>
     <row r="148" ht="13" customHeight="1" spans="1:7">
       <c r="A148" s="6" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="B148"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
-      <c r="F148"/>
+      <c r="F148" s="6" t="s">
+        <v>890</v>
+      </c>
       <c r="G148" s="2" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="149" ht="13" customHeight="1" spans="1:7">
       <c r="A149" s="6" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B149"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
-      <c r="F149" s="6"/>
+      <c r="F149" s="6" t="s">
+        <v>893</v>
+      </c>
       <c r="G149" s="2" t="s">
         <v>894</v>
       </c>
@@ -27444,16 +27465,16 @@
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
-      <c r="F150" s="6"/>
+      <c r="F150"/>
       <c r="G150" s="2" t="s">
         <v>896</v>
       </c>
     </row>
     <row r="151" ht="13" customHeight="1" spans="1:7">
-      <c r="A151" s="6"/>
-      <c r="B151" s="6" t="s">
+      <c r="A151" s="6" t="s">
         <v>897</v>
       </c>
+      <c r="B151"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
@@ -27463,10 +27484,10 @@
       </c>
     </row>
     <row r="152" ht="13" customHeight="1" spans="1:7">
-      <c r="A152" s="6"/>
-      <c r="B152" s="7" t="s">
+      <c r="A152" s="6" t="s">
         <v>899</v>
       </c>
+      <c r="B152"/>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="E152" s="6"/>
@@ -27477,7 +27498,7 @@
     </row>
     <row r="153" ht="13" customHeight="1" spans="1:7">
       <c r="A153" s="6"/>
-      <c r="B153" s="7" t="s">
+      <c r="B153" s="6" t="s">
         <v>901</v>
       </c>
       <c r="C153" s="6"/>
@@ -27503,7 +27524,7 @@
     </row>
     <row r="155" ht="13" customHeight="1" spans="1:7">
       <c r="A155" s="6"/>
-      <c r="B155" s="6" t="s">
+      <c r="B155" s="7" t="s">
         <v>905</v>
       </c>
       <c r="C155" s="6"/>
@@ -27529,7 +27550,7 @@
     </row>
     <row r="157" ht="13" customHeight="1" spans="1:7">
       <c r="A157" s="6"/>
-      <c r="B157" s="7" t="s">
+      <c r="B157" s="6" t="s">
         <v>909</v>
       </c>
       <c r="C157" s="6"/>
@@ -27594,7 +27615,7 @@
     </row>
     <row r="162" ht="13" customHeight="1" spans="1:7">
       <c r="A162" s="6"/>
-      <c r="B162" s="6" t="s">
+      <c r="B162" s="7" t="s">
         <v>919</v>
       </c>
       <c r="C162" s="6"/>
@@ -27607,7 +27628,7 @@
     </row>
     <row r="163" ht="13" customHeight="1" spans="1:7">
       <c r="A163" s="6"/>
-      <c r="B163" s="6" t="s">
+      <c r="B163" s="7" t="s">
         <v>921</v>
       </c>
       <c r="C163" s="6"/>
@@ -27624,7 +27645,7 @@
         <v>923</v>
       </c>
       <c r="C164" s="6"/>
-      <c r="D164"/>
+      <c r="D164" s="6"/>
       <c r="E164" s="6"/>
       <c r="F164" s="6"/>
       <c r="G164" s="2" t="s">
@@ -27633,7 +27654,7 @@
     </row>
     <row r="165" ht="13" customHeight="1" spans="1:7">
       <c r="A165" s="6"/>
-      <c r="B165" s="7" t="s">
+      <c r="B165" s="6" t="s">
         <v>925</v>
       </c>
       <c r="C165" s="6"/>
@@ -27650,7 +27671,7 @@
         <v>927</v>
       </c>
       <c r="C166" s="6"/>
-      <c r="D166" s="6"/>
+      <c r="D166"/>
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
       <c r="G166" s="2" t="s">
@@ -27659,7 +27680,7 @@
     </row>
     <row r="167" ht="13" customHeight="1" spans="1:7">
       <c r="A167" s="6"/>
-      <c r="B167" s="6" t="s">
+      <c r="B167" s="7" t="s">
         <v>929</v>
       </c>
       <c r="C167" s="6"/>
@@ -27672,12 +27693,12 @@
     </row>
     <row r="168" ht="13" customHeight="1" spans="1:7">
       <c r="A168" s="6"/>
-      <c r="B168" s="6"/>
+      <c r="B168" s="6" t="s">
+        <v>931</v>
+      </c>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
-      <c r="E168" s="6" t="s">
-        <v>931</v>
-      </c>
+      <c r="E168" s="6"/>
       <c r="F168" s="6"/>
       <c r="G168" s="2" t="s">
         <v>932</v>
@@ -27685,57 +27706,67 @@
     </row>
     <row r="169" ht="13" customHeight="1" spans="1:7">
       <c r="A169" s="6"/>
-      <c r="B169" s="6"/>
+      <c r="B169" s="6" t="s">
+        <v>933</v>
+      </c>
       <c r="C169" s="6"/>
-      <c r="D169" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E169"/>
-      <c r="F169" s="6" t="s">
-        <v>660</v>
-      </c>
+      <c r="D169" s="6"/>
+      <c r="E169" s="6"/>
+      <c r="F169" s="6"/>
       <c r="G169" s="2" t="s">
-        <v>118</v>
+        <v>934</v>
       </c>
     </row>
     <row r="170" ht="13" customHeight="1" spans="1:7">
-      <c r="A170" s="6" t="s">
-        <v>661</v>
-      </c>
-      <c r="B170" s="6" t="s">
-        <v>933</v>
-      </c>
-      <c r="C170" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="D170" s="6" t="s">
-        <v>126</v>
-      </c>
+      <c r="A170" s="6"/>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
       <c r="E170" s="6" t="s">
-        <v>470</v>
-      </c>
-      <c r="F170" s="6" t="s">
-        <v>125</v>
-      </c>
+        <v>935</v>
+      </c>
+      <c r="F170" s="6"/>
       <c r="G170" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="171" ht="13" customHeight="1" spans="1:6">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="171" ht="13" customHeight="1" spans="1:7">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
-      <c r="D171" s="6"/>
-      <c r="E171" s="6"/>
-      <c r="F171" s="6"/>
-    </row>
-    <row r="172" ht="13" customHeight="1" spans="1:6">
-      <c r="A172" s="6"/>
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="6"/>
-      <c r="F172" s="6"/>
+      <c r="D171" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E171"/>
+      <c r="F171" s="6" t="s">
+        <v>660</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="172" ht="13" customHeight="1" spans="1:7">
+      <c r="A172" s="6" t="s">
+        <v>661</v>
+      </c>
+      <c r="B172" s="6" t="s">
+        <v>937</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E172" s="6" t="s">
+        <v>470</v>
+      </c>
+      <c r="F172" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G172" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="173" ht="13" customHeight="1" spans="1:6">
       <c r="A173" s="6"/>
@@ -27817,8 +27848,24 @@
       <c r="E182" s="6"/>
       <c r="F182" s="6"/>
     </row>
+    <row r="183" ht="13" customHeight="1" spans="1:6">
+      <c r="A183" s="6"/>
+      <c r="B183" s="6"/>
+      <c r="C183" s="6"/>
+      <c r="D183" s="6"/>
+      <c r="E183" s="6"/>
+      <c r="F183" s="6"/>
+    </row>
+    <row r="184" ht="13" customHeight="1" spans="1:6">
+      <c r="A184" s="6"/>
+      <c r="B184" s="6"/>
+      <c r="C184" s="6"/>
+      <c r="D184" s="6"/>
+      <c r="E184" s="6"/>
+      <c r="F184" s="6"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G170"/>
+  <autoFilter ref="A1:G172"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Adjust BancoDoBrasil schema acording normalization
</commit_message>
<xml_diff>
--- a/docs/Normalization.xlsx
+++ b/docs/Normalization.xlsx
@@ -3157,10 +3157,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3196,8 +3196,60 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3211,29 +3263,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3241,22 +3272,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3270,31 +3286,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3308,16 +3316,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3331,10 +3331,17 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3344,15 +3351,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3391,8 +3391,68 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
         <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -3403,7 +3463,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3415,67 +3499,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3487,19 +3511,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3517,7 +3535,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3529,43 +3553,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3578,6 +3572,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3600,17 +3606,41 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3631,16 +3661,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3656,21 +3686,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -3679,156 +3694,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3860,6 +3866,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -8876,7 +8885,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47.2583333333333" style="11"/>
+    <col min="1" max="1" width="47.2583333333333" style="12"/>
     <col min="2" max="2" width="47.7416666666667"/>
     <col min="3" max="3" width="49.2583333333333"/>
   </cols>
@@ -8893,183 +8902,183 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="13" t="s">
         <v>473</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="13" t="s">
         <v>477</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="13" t="s">
         <v>478</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" ht="146.25" spans="1:3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="13" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="13" t="s">
         <v>482</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="13" t="s">
         <v>485</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>486</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
     </row>
     <row r="14" ht="97.5" spans="1:3">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>487</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="13" t="s">
         <v>488</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="13" t="s">
         <v>490</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="13" t="s">
         <v>491</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>492</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="13" t="s">
         <v>493</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
     </row>
     <row r="19" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="13" t="s">
         <v>494</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>497</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="13" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="13" t="s">
         <v>499</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="13" t="s">
         <v>502</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
     </row>
     <row r="24" ht="107.25" spans="1:3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="13" t="s">
         <v>503</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="13" t="s">
         <v>504</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>505</v>
       </c>
     </row>
@@ -9085,90 +9094,90 @@
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="12" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="12" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="12" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="12" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="12" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="12" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="12" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="12" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="12" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="12" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="12" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="12" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="12" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="12" t="s">
         <v>520</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="12" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="12" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="12" t="s">
         <v>523</v>
       </c>
     </row>
@@ -9176,140 +9185,140 @@
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="17" t="s">
         <v>471</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="17" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="12" t="s">
         <v>524</v>
       </c>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12" t="s">
+      <c r="B44" s="13"/>
+      <c r="C44" s="13" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="45" ht="78" spans="1:3">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="12" t="s">
         <v>526</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="14" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="46" ht="29.25" spans="1:3">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="12" t="s">
         <v>529</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B46" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="14" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="12" t="s">
         <v>532</v>
       </c>
-      <c r="B47" s="12" t="s">
+      <c r="B47" s="13" t="s">
         <v>530</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="13" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="48" ht="19.5" spans="1:3">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="12" t="s">
         <v>534</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="13" t="s">
         <v>535</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="14" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="49" ht="19.5" spans="1:3">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="12" t="s">
         <v>537</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="13" t="s">
         <v>538</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="14" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="50" ht="29.25" spans="1:3">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="12" t="s">
         <v>540</v>
       </c>
-      <c r="B50" s="12" t="s">
+      <c r="B50" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="14" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="12" t="s">
         <v>543</v>
       </c>
-      <c r="B51" s="12" t="s">
+      <c r="B51" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="13" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="52" ht="409.5" spans="1:3">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="12" t="s">
         <v>545</v>
       </c>
-      <c r="B52" s="12" t="s">
+      <c r="B52" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="14" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="11" t="s">
+      <c r="A53" s="12" t="s">
         <v>547</v>
       </c>
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="13" t="s">
         <v>527</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="13" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="11" t="s">
+      <c r="A54" s="12" t="s">
         <v>549</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C54" s="12" t="s">
+      <c r="C54" s="13" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>550</v>
       </c>
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="13" t="s">
         <v>541</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="13" t="s">
         <v>544</v>
       </c>
     </row>
@@ -9325,236 +9334,236 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="12" t="s">
         <v>551</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="13" t="s">
         <v>552</v>
       </c>
-      <c r="C57" s="12"/>
+      <c r="C57" s="13"/>
     </row>
     <row r="58" ht="87.75" spans="1:3">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="12" t="s">
         <v>553</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="13"/>
+      <c r="C58" s="14" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="59" ht="107.25" spans="1:3">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="12" t="s">
         <v>555</v>
       </c>
-      <c r="B59" s="12" t="s">
+      <c r="B59" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="C59" s="13" t="s">
+      <c r="C59" s="14" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="12" t="s">
         <v>558</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="12" t="s">
         <v>560</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="C61" s="12" t="s">
+      <c r="C61" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="12" t="s">
         <v>562</v>
       </c>
-      <c r="B62" s="12" t="s">
+      <c r="B62" s="13" t="s">
         <v>563</v>
       </c>
-      <c r="C62" s="12" t="s">
+      <c r="C62" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="12" t="s">
         <v>564</v>
       </c>
-      <c r="B63" s="12" t="s">
+      <c r="B63" s="13" t="s">
         <v>565</v>
       </c>
-      <c r="C63" s="12" t="s">
+      <c r="C63" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="64" ht="97.5" spans="1:3">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>566</v>
       </c>
-      <c r="B64" s="12"/>
-      <c r="C64" s="13" t="s">
+      <c r="B64" s="13"/>
+      <c r="C64" s="14" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="12" t="s">
         <v>568</v>
       </c>
-      <c r="B65" s="12"/>
-      <c r="C65" s="12" t="s">
+      <c r="B65" s="13"/>
+      <c r="C65" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12" t="s">
+      <c r="B66" s="13"/>
+      <c r="C66" s="13" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="67" ht="48.75" spans="1:3">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="12" t="s">
         <v>570</v>
       </c>
-      <c r="B67" s="12"/>
-      <c r="C67" s="13" t="s">
+      <c r="B67" s="13"/>
+      <c r="C67" s="14" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="68" ht="78" spans="1:3">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="12" t="s">
         <v>572</v>
       </c>
-      <c r="B68" s="12"/>
-      <c r="C68" s="13" t="s">
+      <c r="B68" s="13"/>
+      <c r="C68" s="14" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="11" t="s">
+      <c r="A69" s="12" t="s">
         <v>574</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="13" t="s">
         <v>575</v>
       </c>
-      <c r="C69" s="12" t="s">
+      <c r="C69" s="13" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="11" t="s">
+      <c r="A70" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12" t="s">
+      <c r="B70" s="13"/>
+      <c r="C70" s="13" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="71" ht="48.75" spans="1:3">
-      <c r="A71" s="11" t="s">
+      <c r="A71" s="12" t="s">
         <v>579</v>
       </c>
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="13" t="s">
         <v>580</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="14" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="11" t="s">
+      <c r="A72" s="12" t="s">
         <v>582</v>
       </c>
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="13" t="s">
         <v>561</v>
       </c>
-      <c r="C72" s="12" t="s">
+      <c r="C72" s="13" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="73" ht="39" spans="1:3">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="12" t="s">
         <v>583</v>
       </c>
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="13" t="s">
         <v>584</v>
       </c>
-      <c r="C73" s="13" t="s">
+      <c r="C73" s="14" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="12" t="s">
         <v>586</v>
       </c>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12" t="s">
+      <c r="B74" s="13"/>
+      <c r="C74" s="13" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="12" t="s">
         <v>587</v>
       </c>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12" t="s">
+      <c r="B75" s="13"/>
+      <c r="C75" s="13" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="76" ht="97.5" spans="1:3">
-      <c r="A76" s="11" t="s">
+      <c r="A76" s="12" t="s">
         <v>588</v>
       </c>
-      <c r="B76" s="12"/>
-      <c r="C76" s="13" t="s">
+      <c r="B76" s="13"/>
+      <c r="C76" s="14" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="11" t="s">
+      <c r="A77" s="12" t="s">
         <v>590</v>
       </c>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12" t="s">
+      <c r="B77" s="13"/>
+      <c r="C77" s="13" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="78" ht="48.75" spans="1:3">
-      <c r="A78" s="11" t="s">
+      <c r="A78" s="12" t="s">
         <v>591</v>
       </c>
-      <c r="B78" s="12"/>
-      <c r="C78" s="13" t="s">
+      <c r="B78" s="13"/>
+      <c r="C78" s="14" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="79" ht="107.25" spans="1:3">
-      <c r="A79" s="11" t="s">
+      <c r="A79" s="12" t="s">
         <v>593</v>
       </c>
-      <c r="B79" s="12"/>
-      <c r="C79" s="13" t="s">
+      <c r="B79" s="13"/>
+      <c r="C79" s="14" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="80" ht="39" spans="1:3">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="12" t="s">
         <v>595</v>
       </c>
-      <c r="B80" s="12"/>
-      <c r="C80" s="13" t="s">
+      <c r="B80" s="13"/>
+      <c r="C80" s="14" t="s">
         <v>596</v>
       </c>
     </row>
@@ -9570,62 +9579,62 @@
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="12" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="11" t="s">
+      <c r="A83" s="12" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="12" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="12" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="12" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="12" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="12" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="11" t="s">
+      <c r="A89" s="12" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="11" t="s">
+      <c r="A90" s="12" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="12" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="11" t="s">
+      <c r="A92" s="12" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="11" t="s">
+      <c r="A93" s="12" t="s">
         <v>608</v>
       </c>
     </row>
@@ -9641,47 +9650,47 @@
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="11" t="s">
+      <c r="A95" s="12" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="11" t="s">
+      <c r="A96" s="12" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="12" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="11" t="s">
+      <c r="A98" s="12" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="11" t="s">
+      <c r="A99" s="12" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="12" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="11" t="s">
+      <c r="A101" s="12" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="11" t="s">
+      <c r="A102" s="12" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="11" t="s">
+      <c r="A103" s="12" t="s">
         <v>617</v>
       </c>
     </row>
@@ -9704,9 +9713,9 @@
   <dimension ref="A1:AMJ184"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9991,7 +10000,7 @@
       </c>
     </row>
     <row r="15" ht="13" customHeight="1" spans="1:7">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="6" t="s">
         <v>639</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -10832,7 +10841,7 @@
       <c r="H64"/>
     </row>
     <row r="65" ht="13" customHeight="1" spans="1:8">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="10" t="s">
         <v>718</v>
       </c>
       <c r="B65" s="7" t="s">
@@ -13977,7 +13986,7 @@
       <c r="C70" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="11" t="s">
         <v>197</v>
       </c>
       <c r="E70" s="6" t="s">

</xml_diff>

<commit_message>
Midpoint on bradesco return normalization
</commit_message>
<xml_diff>
--- a/docs/Normalization.xlsx
+++ b/docs/Normalization.xlsx
@@ -3052,7 +3052,7 @@
 Títulos baixados</t>
   </si>
   <si>
-    <t>dischargeQuantity</t>
+    <t>dischargedQuantity</t>
   </si>
   <si>
     <t>Valor dos Registros –
@@ -3060,7 +3060,7 @@
 Títulos baixados</t>
   </si>
   <si>
-    <t>valueQuantity</t>
+    <t>dischargedValue</t>
   </si>
   <si>
     <t>Quantidade de registros
@@ -3071,7 +3071,7 @@
 Abatimento Cancelado</t>
   </si>
   <si>
-    <t>rebateCancelQuantity</t>
+    <t>rebateCanceledQuantity</t>
   </si>
   <si>
     <t>Valor dos Registros –
@@ -3079,7 +3079,7 @@
 Abatimento Cancelado</t>
   </si>
   <si>
-    <t>rebateCancelValue</t>
+    <t>rebateCanceledValue</t>
   </si>
   <si>
     <t>Quantidade dos Registros
@@ -3090,7 +3090,7 @@
 Vencimento Alterado</t>
   </si>
   <si>
-    <t>rebateUpdateQuantity</t>
+    <t>expirationUpdatedQuantity</t>
   </si>
   <si>
     <t>Valor dos Registros –
@@ -3100,25 +3100,25 @@
 Vencimento Alterado</t>
   </si>
   <si>
-    <t>rebateUpdateValue</t>
+    <t>expirationUpdatedValue</t>
   </si>
   <si>
     <t>Quantidade dos Registros-Ocorrência 12 - Abatimento Concedido</t>
   </si>
   <si>
-    <t>rebateQuantity</t>
+    <t>rebatedQuantity</t>
   </si>
   <si>
     <t>Valor dos Registros - Ocorência 12 - Abatimento Concedido</t>
   </si>
   <si>
-    <t>rebateValue</t>
+    <t>rebatedValue</t>
   </si>
   <si>
     <t>Quantidade dos Registros - Ocorrência 19 -  Confirmação Da Instrução de protesto</t>
   </si>
   <si>
-    <t>protestQuantity</t>
+    <t>protestedQuantity</t>
   </si>
   <si>
     <t>Valor dos Registros –
@@ -3128,7 +3128,7 @@
 de Protesto</t>
   </si>
   <si>
-    <t>protestValue</t>
+    <t>protestedValue</t>
   </si>
   <si>
     <t>Valor Total dos Rateios Efetuados</t>
@@ -3157,9 +3157,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -3205,7 +3205,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3218,48 +3218,18 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3270,9 +3240,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3286,23 +3271,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3324,7 +3294,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3332,7 +3302,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3340,13 +3347,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3403,7 +3403,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3415,7 +3427,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3427,37 +3517,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3469,67 +3565,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3541,49 +3583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3599,8 +3599,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3610,22 +3612,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3646,21 +3648,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -3675,13 +3662,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3694,140 +3685,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -9713,15 +9713,15 @@
   <dimension ref="A1:AMJ184"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="15.2583333333333" style="1"/>
-    <col min="2" max="2" width="20.625" style="1"/>
+    <col min="2" max="2" width="19.8583333333333" style="1" customWidth="1"/>
     <col min="3" max="4" width="16.775" style="1"/>
     <col min="5" max="6" width="20.625" style="1"/>
     <col min="7" max="7" width="17.7416666666667" style="2"/>

</xml_diff>

<commit_message>
Midpoint on Bradesco returning
</commit_message>
<xml_diff>
--- a/docs/Normalization.xlsx
+++ b/docs/Normalization.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939">
   <si>
     <t>Banco do Brasil</t>
   </si>
@@ -2472,7 +2472,12 @@
 de Instrução de Protesto)</t>
   </si>
   <si>
-    <t>eventCode25</t>
+    <t>protestMotive</t>
+  </si>
+  <si>
+    <t>Identificação da
+Empresa Beneficiário
+no Banco</t>
   </si>
   <si>
     <t>Indicador de Rateio
@@ -3157,10 +3162,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -3212,12 +3217,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3225,16 +3232,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3247,11 +3251,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3271,35 +3274,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -3309,13 +3283,14 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -3330,9 +3305,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3346,7 +3335,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3403,7 +3408,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3433,7 +3444,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3445,25 +3492,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3481,13 +3510,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3505,49 +3546,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3559,31 +3582,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3597,22 +3602,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3647,21 +3647,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3680,8 +3665,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3694,139 +3679,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="38" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -3834,7 +3839,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3867,6 +3872,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -8885,7 +8893,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47.2583333333333" style="12"/>
+    <col min="1" max="1" width="47.2583333333333" style="13"/>
     <col min="2" max="2" width="47.7416666666667"/>
     <col min="3" max="3" width="49.2583333333333"/>
   </cols>
@@ -8902,183 +8910,183 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>473</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>474</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="14" t="s">
         <v>475</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="14" t="s">
         <v>476</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="14" t="s">
         <v>477</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="14" t="s">
         <v>478</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>479</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="14" t="s">
         <v>480</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" ht="146.25" spans="1:3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>481</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>482</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>485</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>486</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
     </row>
     <row r="14" ht="97.5" spans="1:3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>487</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>488</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="14" t="s">
         <v>490</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="14" t="s">
         <v>491</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
     </row>
     <row r="19" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="17" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" ht="12.75" customHeight="1" spans="1:3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>500</v>
       </c>
-      <c r="C22" s="16" t="s">
+      <c r="C22" s="17" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>502</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
     </row>
     <row r="24" ht="107.25" spans="1:3">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="14" t="s">
         <v>503</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>505</v>
       </c>
     </row>
@@ -9094,90 +9102,90 @@
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="13" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="13" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="13" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="13" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="13" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="12" t="s">
+      <c r="A34" s="13" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="13" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="13" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="12" t="s">
+      <c r="A37" s="13" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="13" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="13" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:2">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="13" t="s">
         <v>520</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="13" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="13" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="13" t="s">
         <v>523</v>
       </c>
     </row>
@@ -9185,140 +9193,140 @@
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="18" t="s">
         <v>471</v>
       </c>
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="18" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="44" spans="1:3">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="13" t="s">
         <v>524</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13" t="s">
+      <c r="B44" s="14"/>
+      <c r="C44" s="14" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="45" ht="78" spans="1:3">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="13" t="s">
         <v>526</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" s="15" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="46" ht="29.25" spans="1:3">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="13" t="s">
         <v>529</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C46" s="15" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:3">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="13" t="s">
         <v>532</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="14" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="48" ht="19.5" spans="1:3">
-      <c r="A48" s="12" t="s">
+      <c r="A48" s="13" t="s">
         <v>534</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="C48" s="15" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="49" ht="19.5" spans="1:3">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="13" t="s">
         <v>537</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="C49" s="14" t="s">
+      <c r="C49" s="15" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="50" ht="29.25" spans="1:3">
-      <c r="A50" s="12" t="s">
+      <c r="A50" s="13" t="s">
         <v>540</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" s="15" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="51" spans="1:3">
-      <c r="A51" s="12" t="s">
+      <c r="A51" s="13" t="s">
         <v>543</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="14" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="52" ht="409.5" spans="1:3">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="13" t="s">
         <v>545</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="C52" s="14" t="s">
+      <c r="C52" s="15" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="53" spans="1:3">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="13" t="s">
         <v>547</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="14" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3">
-      <c r="A54" s="12" t="s">
+      <c r="A54" s="13" t="s">
         <v>549</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="14" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="12" t="s">
+      <c r="A55" s="13" t="s">
         <v>550</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="14" t="s">
         <v>544</v>
       </c>
     </row>
@@ -9334,236 +9342,236 @@
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="12" t="s">
+      <c r="A57" s="13" t="s">
         <v>551</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="14" t="s">
         <v>552</v>
       </c>
-      <c r="C57" s="13"/>
+      <c r="C57" s="14"/>
     </row>
     <row r="58" ht="87.75" spans="1:3">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="13" t="s">
         <v>553</v>
       </c>
-      <c r="B58" s="13"/>
-      <c r="C58" s="14" t="s">
+      <c r="B58" s="14"/>
+      <c r="C58" s="15" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="59" ht="107.25" spans="1:3">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="13" t="s">
         <v>555</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="14" t="s">
         <v>556</v>
       </c>
-      <c r="C59" s="14" t="s">
+      <c r="C59" s="15" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:3">
-      <c r="A60" s="12" t="s">
+      <c r="A60" s="13" t="s">
         <v>558</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="14" t="s">
         <v>556</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="C60" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="61" spans="1:3">
-      <c r="A61" s="12" t="s">
+      <c r="A61" s="13" t="s">
         <v>560</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="14" t="s">
         <v>561</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="62" spans="1:3">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="13" t="s">
         <v>562</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="14" t="s">
         <v>563</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="C62" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="13" t="s">
         <v>564</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="14" t="s">
         <v>565</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C63" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="64" ht="97.5" spans="1:3">
-      <c r="A64" s="12" t="s">
+      <c r="A64" s="13" t="s">
         <v>566</v>
       </c>
-      <c r="B64" s="13"/>
-      <c r="C64" s="14" t="s">
+      <c r="B64" s="14"/>
+      <c r="C64" s="15" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="65" spans="1:3">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="13" t="s">
         <v>568</v>
       </c>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13" t="s">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="13" t="s">
         <v>569</v>
       </c>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13" t="s">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="67" ht="48.75" spans="1:3">
-      <c r="A67" s="12" t="s">
+      <c r="A67" s="13" t="s">
         <v>570</v>
       </c>
-      <c r="B67" s="13"/>
-      <c r="C67" s="14" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="15" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="68" ht="78" spans="1:3">
-      <c r="A68" s="12" t="s">
+      <c r="A68" s="13" t="s">
         <v>572</v>
       </c>
-      <c r="B68" s="13"/>
-      <c r="C68" s="14" t="s">
+      <c r="B68" s="14"/>
+      <c r="C68" s="15" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" s="12" t="s">
+      <c r="A69" s="13" t="s">
         <v>574</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="14" t="s">
         <v>575</v>
       </c>
-      <c r="C69" s="13" t="s">
+      <c r="C69" s="14" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="70" spans="1:3">
-      <c r="A70" s="12" t="s">
+      <c r="A70" s="13" t="s">
         <v>577</v>
       </c>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13" t="s">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="71" ht="48.75" spans="1:3">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="13" t="s">
         <v>579</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="14" t="s">
         <v>580</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C71" s="15" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="12" t="s">
+      <c r="A72" s="13" t="s">
         <v>582</v>
       </c>
-      <c r="B72" s="13" t="s">
+      <c r="B72" s="14" t="s">
         <v>561</v>
       </c>
-      <c r="C72" s="13" t="s">
+      <c r="C72" s="14" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="73" ht="39" spans="1:3">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="13" t="s">
         <v>583</v>
       </c>
-      <c r="B73" s="13" t="s">
+      <c r="B73" s="14" t="s">
         <v>584</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C73" s="15" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="12" t="s">
+      <c r="A74" s="13" t="s">
         <v>586</v>
       </c>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13" t="s">
+      <c r="B74" s="14"/>
+      <c r="C74" s="14" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="12" t="s">
+      <c r="A75" s="13" t="s">
         <v>587</v>
       </c>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13" t="s">
+      <c r="B75" s="14"/>
+      <c r="C75" s="14" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="76" ht="97.5" spans="1:3">
-      <c r="A76" s="12" t="s">
+      <c r="A76" s="13" t="s">
         <v>588</v>
       </c>
-      <c r="B76" s="13"/>
-      <c r="C76" s="14" t="s">
+      <c r="B76" s="14"/>
+      <c r="C76" s="15" t="s">
         <v>589</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="12" t="s">
+      <c r="A77" s="13" t="s">
         <v>590</v>
       </c>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13" t="s">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="78" ht="48.75" spans="1:3">
-      <c r="A78" s="12" t="s">
+      <c r="A78" s="13" t="s">
         <v>591</v>
       </c>
-      <c r="B78" s="13"/>
-      <c r="C78" s="14" t="s">
+      <c r="B78" s="14"/>
+      <c r="C78" s="15" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="79" ht="107.25" spans="1:3">
-      <c r="A79" s="12" t="s">
+      <c r="A79" s="13" t="s">
         <v>593</v>
       </c>
-      <c r="B79" s="13"/>
-      <c r="C79" s="14" t="s">
+      <c r="B79" s="14"/>
+      <c r="C79" s="15" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="80" ht="39" spans="1:3">
-      <c r="A80" s="12" t="s">
+      <c r="A80" s="13" t="s">
         <v>595</v>
       </c>
-      <c r="B80" s="13"/>
-      <c r="C80" s="14" t="s">
+      <c r="B80" s="14"/>
+      <c r="C80" s="15" t="s">
         <v>596</v>
       </c>
     </row>
@@ -9579,62 +9587,62 @@
       </c>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="13" t="s">
         <v>597</v>
       </c>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="13" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="13" t="s">
         <v>599</v>
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="13" t="s">
         <v>600</v>
       </c>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="13" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="12" t="s">
+      <c r="A87" s="13" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="13" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="13" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="12" t="s">
+      <c r="A90" s="13" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="12" t="s">
+      <c r="A91" s="13" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="12" t="s">
+      <c r="A92" s="13" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="12" t="s">
+      <c r="A93" s="13" t="s">
         <v>608</v>
       </c>
     </row>
@@ -9650,47 +9658,47 @@
       </c>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="12" t="s">
+      <c r="A95" s="13" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="12" t="s">
+      <c r="A96" s="13" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="12" t="s">
+      <c r="A97" s="13" t="s">
         <v>611</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="12" t="s">
+      <c r="A98" s="13" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="12" t="s">
+      <c r="A99" s="13" t="s">
         <v>613</v>
       </c>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="12" t="s">
+      <c r="A100" s="13" t="s">
         <v>614</v>
       </c>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="12" t="s">
+      <c r="A101" s="13" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="12" t="s">
+      <c r="A102" s="13" t="s">
         <v>616</v>
       </c>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="12" t="s">
+      <c r="A103" s="13" t="s">
         <v>617</v>
       </c>
     </row>
@@ -9713,9 +9721,9 @@
   <dimension ref="A1:AMJ184"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G166" sqref="G166"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -10878,7 +10886,9 @@
     </row>
     <row r="67" ht="13" customHeight="1" spans="1:1024">
       <c r="A67"/>
-      <c r="B67" s="6"/>
+      <c r="B67" s="11" t="s">
+        <v>726</v>
+      </c>
       <c r="C67" s="6" t="s">
         <v>86</v>
       </c>
@@ -11909,7 +11919,7 @@
     <row r="68" ht="13" customHeight="1" spans="1:1024">
       <c r="A68" s="6"/>
       <c r="B68" s="7" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="C68"/>
       <c r="D68"/>
@@ -12938,16 +12948,16 @@
     </row>
     <row r="69" ht="13" customHeight="1" spans="1:1024">
       <c r="A69" s="6" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>360</v>
@@ -13981,16 +13991,16 @@
         <v>197</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="C70" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="D70" s="12" t="s">
         <v>197</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>196</v>
@@ -15030,10 +15040,10 @@
         <v>203</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>203</v>
@@ -16061,7 +16071,7 @@
         <v>639</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="C72" s="6" t="s">
         <v>210</v>
@@ -16070,10 +16080,10 @@
         <v>210</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>210</v>
@@ -17101,7 +17111,7 @@
         <v>49</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C73" s="6" t="s">
         <v>216</v>
@@ -17110,10 +17120,10 @@
         <v>216</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>216</v>
@@ -18143,10 +18153,10 @@
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74" s="6" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="F74"/>
       <c r="G74" s="2" t="s">
@@ -19175,7 +19185,7 @@
         <v>225</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C75" s="6" t="s">
         <v>225</v>
@@ -20212,7 +20222,7 @@
     </row>
     <row r="76" ht="13" customHeight="1" spans="1:1024">
       <c r="A76" s="6" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>655</v>
@@ -20224,10 +20234,10 @@
         <v>656</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>656</v>
@@ -21252,25 +21262,25 @@
     </row>
     <row r="77" ht="13" customHeight="1" spans="1:1024">
       <c r="A77" s="6" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="E77" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>751</v>
+      </c>
+      <c r="G77" s="2" t="s">
         <v>749</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>750</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>748</v>
       </c>
       <c r="H77"/>
       <c r="I77"/>
@@ -22292,21 +22302,21 @@
     </row>
     <row r="78" ht="13" customHeight="1" spans="1:1024">
       <c r="A78" s="6" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C78"/>
       <c r="D78"/>
       <c r="E78" s="6" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="H78"/>
       <c r="I78"/>
@@ -23328,10 +23338,10 @@
     </row>
     <row r="79" ht="13" customHeight="1" spans="1:1024">
       <c r="A79" s="6" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>277</v>
@@ -23340,10 +23350,10 @@
         <v>277</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>277</v>
@@ -24371,7 +24381,7 @@
         <v>284</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>284</v>
@@ -24380,10 +24390,10 @@
         <v>284</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>284</v>
@@ -25411,7 +25421,7 @@
         <v>270</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>270</v>
@@ -25420,10 +25430,10 @@
         <v>270</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>270</v>
@@ -26448,69 +26458,69 @@
     </row>
     <row r="82" ht="13" customHeight="1" spans="1:7">
       <c r="A82" s="6" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B82"/>
       <c r="C82"/>
       <c r="D82"/>
       <c r="E82" s="6" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="F82"/>
       <c r="G82" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="83" ht="13" customHeight="1" spans="1:7">
       <c r="A83" s="6" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="E83" s="6" t="s">
+        <v>773</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>774</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>772</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>773</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="84" ht="13" customHeight="1" spans="1:7">
       <c r="A84" s="6" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C84" s="6" t="s">
+        <v>777</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>778</v>
+      </c>
+      <c r="E84" s="6" t="s">
         <v>776</v>
       </c>
-      <c r="D84" s="6" t="s">
-        <v>777</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>775</v>
-      </c>
       <c r="F84" s="6" t="s">
+        <v>779</v>
+      </c>
+      <c r="G84" s="2" t="s">
         <v>778</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="85" ht="13" customHeight="1" spans="1:7">
       <c r="A85" s="6"/>
       <c r="B85" s="7" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>439</v>
@@ -26518,7 +26528,7 @@
       <c r="D85" s="6"/>
       <c r="E85" s="6"/>
       <c r="F85" s="6" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>439</v>
@@ -26526,85 +26536,85 @@
     </row>
     <row r="86" ht="13" customHeight="1" spans="1:7">
       <c r="A86" s="6" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="C86"/>
       <c r="D86" s="6" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="E86" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>786</v>
+      </c>
+      <c r="G86" s="2" t="s">
         <v>784</v>
-      </c>
-      <c r="F86" s="6" t="s">
-        <v>785</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>783</v>
       </c>
     </row>
     <row r="87" ht="13" customHeight="1" spans="1:7">
       <c r="A87" s="6" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87"/>
       <c r="D87" s="6"/>
       <c r="E87" s="6" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="F87" s="6"/>
       <c r="G87" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
     </row>
     <row r="88" ht="13" customHeight="1" spans="1:7">
       <c r="A88" s="6" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88"/>
       <c r="D88" s="6"/>
       <c r="E88" s="6" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="F88" s="6"/>
       <c r="G88" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
     </row>
     <row r="89" ht="13" customHeight="1" spans="1:7">
       <c r="A89" s="6" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89"/>
       <c r="D89" s="6"/>
       <c r="E89" s="6" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="F89" s="6"/>
       <c r="G89" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
     </row>
     <row r="90" ht="13" customHeight="1" spans="1:7">
       <c r="A90" s="6" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B90" s="6"/>
       <c r="C90"/>
       <c r="D90" s="6"/>
       <c r="E90" s="6" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
     <row r="91" ht="13" customHeight="1" spans="1:7">
@@ -26614,10 +26624,10 @@
       <c r="D91" s="6"/>
       <c r="E91" s="6"/>
       <c r="F91" s="6" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
     </row>
     <row r="92" ht="13" customHeight="1" spans="1:7">
@@ -26627,7 +26637,7 @@
       <c r="D92"/>
       <c r="E92"/>
       <c r="F92" s="6" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>231</v>
@@ -26650,22 +26660,22 @@
     </row>
     <row r="94" ht="13" customHeight="1" spans="1:7">
       <c r="A94" s="6" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B94"/>
       <c r="C94"/>
       <c r="D94"/>
       <c r="E94" s="6" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F94" s="6"/>
       <c r="G94" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
     <row r="95" ht="13" customHeight="1" spans="1:7">
       <c r="A95" s="6" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B95"/>
       <c r="C95"/>
@@ -26673,13 +26683,13 @@
       <c r="E95"/>
       <c r="F95" s="6"/>
       <c r="G95" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
     </row>
     <row r="96" ht="13" customHeight="1" spans="1:7">
       <c r="A96"/>
       <c r="B96" s="7" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C96"/>
       <c r="D96"/>
@@ -26692,92 +26702,92 @@
     <row r="97" ht="13" customHeight="1" spans="1:7">
       <c r="A97"/>
       <c r="B97" s="6" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C97"/>
       <c r="D97"/>
       <c r="E97"/>
       <c r="F97" s="6"/>
       <c r="G97" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
     </row>
     <row r="98" ht="13" customHeight="1" spans="1:7">
       <c r="A98"/>
       <c r="B98" s="6" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C98"/>
       <c r="D98"/>
       <c r="E98"/>
       <c r="F98" s="6"/>
       <c r="G98" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
     </row>
     <row r="99" ht="13" customHeight="1" spans="1:7">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99" s="6" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="D99"/>
       <c r="E99"/>
       <c r="F99" s="6"/>
       <c r="G99" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
     </row>
     <row r="100" ht="13" customHeight="1" spans="1:7">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100" s="6" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="D100"/>
       <c r="E100"/>
       <c r="F100"/>
       <c r="G100" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
     </row>
     <row r="101" ht="13" customHeight="1" spans="1:7">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101" s="6" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="D101"/>
       <c r="E101"/>
       <c r="F101"/>
       <c r="G101" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
     </row>
     <row r="102" ht="13" customHeight="1" spans="1:7">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102" s="6" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D102"/>
       <c r="E102"/>
       <c r="F102"/>
       <c r="G102" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
     <row r="103" ht="13" customHeight="1" spans="1:7">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103" s="6" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D103"/>
       <c r="E103"/>
       <c r="F103"/>
       <c r="G103" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
     </row>
     <row r="104" ht="13" customHeight="1" spans="1:7">
@@ -26799,7 +26809,7 @@
       <c r="C105" s="6"/>
       <c r="D105"/>
       <c r="E105" s="6" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="F105" s="6"/>
       <c r="G105" s="2" t="s">
@@ -26813,10 +26823,10 @@
       <c r="D106" s="6"/>
       <c r="E106"/>
       <c r="F106" s="6" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="G106" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
     </row>
     <row r="107" ht="13" customHeight="1" spans="1:7">
@@ -26826,10 +26836,10 @@
       <c r="D107" s="6"/>
       <c r="E107"/>
       <c r="F107" s="6" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="G107" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
     </row>
     <row r="108" ht="13" customHeight="1" spans="1:7">
@@ -26881,7 +26891,7 @@
         <v>415</v>
       </c>
       <c r="G111" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
     </row>
     <row r="112" ht="13" customHeight="1" spans="1:7">
@@ -26889,12 +26899,12 @@
       <c r="B112" s="6"/>
       <c r="C112"/>
       <c r="D112" s="6" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="E112" s="6"/>
       <c r="F112"/>
       <c r="G112" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
     </row>
     <row r="113" ht="13" customHeight="1" spans="1:7">
@@ -26902,12 +26912,12 @@
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="E113" s="6"/>
       <c r="F113" s="6"/>
       <c r="G113" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
     </row>
     <row r="114" ht="13" customHeight="1" spans="1:7">
@@ -26915,12 +26925,12 @@
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="E114" s="6"/>
       <c r="F114" s="6"/>
       <c r="G114" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
     </row>
     <row r="115" ht="13" customHeight="1" spans="1:7">
@@ -26928,31 +26938,31 @@
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="E115" s="6"/>
       <c r="F115" s="6"/>
       <c r="G115" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
     </row>
     <row r="116" ht="13" customHeight="1" spans="1:7">
       <c r="A116" s="6" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B116" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="C116" s="6" t="s">
         <v>829</v>
       </c>
-      <c r="C116" s="6" t="s">
-        <v>828</v>
-      </c>
       <c r="D116" s="6" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="E116" s="6"/>
       <c r="F116" s="6"/>
       <c r="G116" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
     </row>
     <row r="117" ht="13" customHeight="1" spans="1:7">
@@ -26965,7 +26975,7 @@
         <v>660</v>
       </c>
       <c r="G117" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
     </row>
     <row r="118" ht="13" customHeight="1" spans="1:7">
@@ -26973,7 +26983,7 @@
         <v>661</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="C118" s="6" t="s">
         <v>126</v>
@@ -27016,7 +27026,7 @@
         <v>17</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="F120" s="6" t="s">
         <v>16</v>
@@ -27027,10 +27037,10 @@
     </row>
     <row r="121" ht="13" customHeight="1" spans="1:7">
       <c r="A121" s="6" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>622</v>
@@ -27039,10 +27049,10 @@
         <v>622</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>622</v>
@@ -27050,10 +27060,10 @@
     </row>
     <row r="122" ht="13" customHeight="1" spans="1:7">
       <c r="A122" s="6" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="C122" s="6" t="s">
         <v>37</v>
@@ -27071,7 +27081,7 @@
     </row>
     <row r="123" ht="13" customHeight="1" spans="1:7">
       <c r="A123" s="6" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B123" s="6" t="s">
         <v>99</v>
@@ -27098,7 +27108,7 @@
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
       <c r="E124" s="6" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="F124" s="6"/>
       <c r="G124" s="2" t="s">
@@ -27111,11 +27121,11 @@
       <c r="C125"/>
       <c r="D125"/>
       <c r="E125" s="6" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="F125"/>
       <c r="G125" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
     </row>
     <row r="126" ht="13" customHeight="1" spans="1:7">
@@ -27124,7 +27134,7 @@
       <c r="C126" s="6"/>
       <c r="D126"/>
       <c r="E126" s="6" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="F126"/>
       <c r="G126" s="2" t="s">
@@ -27137,7 +27147,7 @@
       <c r="C127" s="6"/>
       <c r="D127"/>
       <c r="E127" s="6" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="F127"/>
       <c r="G127" s="2" t="s">
@@ -27150,7 +27160,7 @@
       <c r="C128" s="6"/>
       <c r="D128"/>
       <c r="E128" s="6" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="F128"/>
       <c r="G128" s="2" t="s">
@@ -27163,7 +27173,7 @@
       <c r="C129" s="6"/>
       <c r="D129"/>
       <c r="E129" s="6" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="F129"/>
       <c r="G129" s="2" t="s">
@@ -27176,7 +27186,7 @@
       <c r="C130" s="6"/>
       <c r="D130"/>
       <c r="E130" s="6" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="F130"/>
       <c r="G130" s="2" t="s">
@@ -27189,24 +27199,24 @@
       <c r="C131" s="6"/>
       <c r="D131"/>
       <c r="E131" s="6" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="F131"/>
       <c r="G131" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
     </row>
     <row r="132" ht="13" customHeight="1" spans="1:7">
       <c r="A132"/>
       <c r="B132" s="7" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="C132" s="6"/>
       <c r="D132" s="6" t="s">
         <v>459</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="F132"/>
       <c r="G132" s="2" t="s">
@@ -27216,7 +27226,7 @@
     <row r="133" ht="13" customHeight="1" spans="1:7">
       <c r="A133"/>
       <c r="B133" s="6" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C133" s="6"/>
       <c r="D133" s="6" t="s">
@@ -27231,110 +27241,110 @@
     <row r="134" ht="13" customHeight="1" spans="1:7">
       <c r="A134"/>
       <c r="B134" s="6" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C134" s="6"/>
       <c r="D134" s="6"/>
       <c r="E134" s="6"/>
       <c r="F134"/>
       <c r="G134" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="135" ht="13" customHeight="1" spans="1:7">
       <c r="A135" s="6" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="B135"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="E135"/>
       <c r="F135" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="G135" s="2" t="s">
         <v>858</v>
-      </c>
-      <c r="G135" s="2" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="136" ht="13" customHeight="1" spans="1:7">
       <c r="A136" s="6" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B136"/>
       <c r="C136" s="6"/>
       <c r="D136" s="6" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E136"/>
       <c r="F136" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="G136" s="2" t="s">
         <v>861</v>
-      </c>
-      <c r="G136" s="2" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="137" ht="13" customHeight="1" spans="1:7">
       <c r="A137" s="6" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B137"/>
       <c r="C137" s="6"/>
       <c r="D137" s="6" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="E137" s="6"/>
       <c r="F137" s="6" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="G137" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
     </row>
     <row r="138" ht="13" customHeight="1" spans="1:7">
       <c r="A138" s="6" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B138"/>
       <c r="C138" s="6"/>
       <c r="D138" s="6" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="E138" s="6"/>
       <c r="F138"/>
       <c r="G138" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
     </row>
     <row r="139" ht="13" customHeight="1" spans="1:7">
       <c r="A139" s="6" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B139"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="E139" s="6"/>
       <c r="F139"/>
       <c r="G139" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
     </row>
     <row r="140" ht="13" customHeight="1" spans="1:7">
       <c r="A140" s="6" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B140"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="E140" s="6"/>
       <c r="F140"/>
       <c r="G140" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
     </row>
     <row r="141" ht="13" customHeight="1" spans="1:7">
@@ -27342,12 +27352,12 @@
       <c r="B141"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="E141" s="6"/>
       <c r="F141"/>
       <c r="G141" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
     </row>
     <row r="142" ht="13" customHeight="1" spans="1:7">
@@ -27355,12 +27365,12 @@
       <c r="B142"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="E142" s="6"/>
       <c r="F142"/>
       <c r="G142" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
     </row>
     <row r="143" ht="13" customHeight="1" spans="1:7">
@@ -27368,107 +27378,107 @@
       <c r="B143"/>
       <c r="C143" s="6"/>
       <c r="D143" s="6" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="E143" s="6"/>
       <c r="F143"/>
       <c r="G143" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
     <row r="144" ht="13" customHeight="1" spans="1:7">
       <c r="A144" s="6" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B144"/>
       <c r="C144" s="6"/>
       <c r="D144"/>
       <c r="E144" s="6"/>
       <c r="F144" s="6" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="G144" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
     </row>
     <row r="145" ht="13" customHeight="1" spans="1:7">
       <c r="A145" s="6" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="B145"/>
       <c r="C145" s="6"/>
       <c r="D145"/>
       <c r="E145" s="6"/>
       <c r="F145" s="6" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
     <row r="146" ht="13" customHeight="1" spans="1:7">
       <c r="A146" s="6" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="B146"/>
       <c r="C146" s="6"/>
       <c r="D146"/>
       <c r="E146" s="6"/>
       <c r="F146" s="6" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="G146" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
     </row>
     <row r="147" ht="13" customHeight="1" spans="1:7">
       <c r="A147" s="6" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="B147"/>
       <c r="C147" s="6"/>
       <c r="D147" s="6"/>
       <c r="E147" s="6"/>
       <c r="F147" s="6" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
     </row>
     <row r="148" ht="13" customHeight="1" spans="1:7">
       <c r="A148" s="6" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B148"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
       <c r="F148" s="6" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="G148" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
     <row r="149" ht="13" customHeight="1" spans="1:7">
       <c r="A149" s="6" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B149"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
       <c r="F149" s="6" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
     <row r="150" ht="13" customHeight="1" spans="1:7">
       <c r="A150" s="6" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B150"/>
       <c r="C150" s="6"/>
@@ -27476,12 +27486,12 @@
       <c r="E150" s="6"/>
       <c r="F150"/>
       <c r="G150" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
     </row>
     <row r="151" ht="13" customHeight="1" spans="1:7">
       <c r="A151" s="6" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="B151"/>
       <c r="C151" s="6"/>
@@ -27489,12 +27499,12 @@
       <c r="E151" s="6"/>
       <c r="F151" s="6"/>
       <c r="G151" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="152" ht="13" customHeight="1" spans="1:7">
       <c r="A152" s="6" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="B152"/>
       <c r="C152" s="6"/>
@@ -27502,228 +27512,228 @@
       <c r="E152" s="6"/>
       <c r="F152" s="6"/>
       <c r="G152" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="153" ht="13" customHeight="1" spans="1:7">
       <c r="A153" s="6"/>
       <c r="B153" s="6" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="C153" s="6"/>
       <c r="D153" s="6"/>
       <c r="E153" s="6"/>
       <c r="F153" s="6"/>
       <c r="G153" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="154" ht="13" customHeight="1" spans="1:7">
       <c r="A154" s="6"/>
       <c r="B154" s="7" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C154" s="6"/>
       <c r="D154" s="6"/>
       <c r="E154" s="6"/>
       <c r="F154" s="6"/>
       <c r="G154" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="155" ht="13" customHeight="1" spans="1:7">
       <c r="A155" s="6"/>
       <c r="B155" s="7" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="C155" s="6"/>
       <c r="D155" s="6"/>
       <c r="E155" s="6"/>
       <c r="F155" s="6"/>
       <c r="G155" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="156" ht="13" customHeight="1" spans="1:7">
       <c r="A156" s="6"/>
       <c r="B156" s="7" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="C156" s="6"/>
       <c r="D156" s="6"/>
       <c r="E156" s="6"/>
       <c r="F156" s="6"/>
       <c r="G156" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row r="157" ht="13" customHeight="1" spans="1:7">
       <c r="A157" s="6"/>
       <c r="B157" s="6" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="E157" s="6"/>
       <c r="F157" s="6"/>
       <c r="G157" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="158" ht="13" customHeight="1" spans="1:7">
       <c r="A158" s="6"/>
       <c r="B158" s="7" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
       <c r="F158" s="6"/>
       <c r="G158" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="159" ht="13" customHeight="1" spans="1:7">
       <c r="A159" s="6"/>
       <c r="B159" s="7" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="6"/>
       <c r="F159" s="6"/>
       <c r="G159" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="160" ht="13" customHeight="1" spans="1:7">
       <c r="A160" s="6"/>
       <c r="B160" s="7" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="E160" s="6"/>
       <c r="F160" s="6"/>
       <c r="G160" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="161" ht="13" customHeight="1" spans="1:7">
       <c r="A161" s="6"/>
       <c r="B161" s="7" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C161" s="6"/>
       <c r="D161" s="6"/>
       <c r="E161" s="6"/>
       <c r="F161" s="6"/>
       <c r="G161" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row r="162" ht="13" customHeight="1" spans="1:7">
       <c r="A162" s="6"/>
       <c r="B162" s="7" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="C162" s="6"/>
       <c r="D162" s="6"/>
       <c r="E162" s="6"/>
       <c r="F162" s="6"/>
       <c r="G162" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
     <row r="163" ht="13" customHeight="1" spans="1:7">
       <c r="A163" s="6"/>
       <c r="B163" s="7" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
       <c r="E163" s="6"/>
       <c r="F163" s="6"/>
       <c r="G163" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="164" ht="13" customHeight="1" spans="1:7">
       <c r="A164" s="6"/>
       <c r="B164" s="6" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C164" s="6"/>
       <c r="D164" s="6"/>
       <c r="E164" s="6"/>
       <c r="F164" s="6"/>
       <c r="G164" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="165" ht="13" customHeight="1" spans="1:7">
       <c r="A165" s="6"/>
       <c r="B165" s="6" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="C165" s="6"/>
       <c r="D165" s="6"/>
       <c r="E165" s="6"/>
       <c r="F165" s="6"/>
       <c r="G165" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row r="166" ht="13" customHeight="1" spans="1:7">
       <c r="A166" s="6"/>
       <c r="B166" s="6" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="C166" s="6"/>
       <c r="D166"/>
       <c r="E166" s="6"/>
       <c r="F166" s="6"/>
       <c r="G166" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="167" ht="13" customHeight="1" spans="1:7">
       <c r="A167" s="6"/>
       <c r="B167" s="7" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="E167" s="6"/>
       <c r="F167" s="6"/>
       <c r="G167" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="168" ht="13" customHeight="1" spans="1:7">
       <c r="A168" s="6"/>
       <c r="B168" s="6" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="E168" s="6"/>
       <c r="F168" s="6"/>
       <c r="G168" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="169" ht="13" customHeight="1" spans="1:7">
       <c r="A169" s="6"/>
       <c r="B169" s="6" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="E169" s="6"/>
       <c r="F169" s="6"/>
       <c r="G169" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="170" ht="13" customHeight="1" spans="1:7">
@@ -27732,11 +27742,11 @@
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
       <c r="E170" s="6" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="F170" s="6"/>
       <c r="G170" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="171" ht="13" customHeight="1" spans="1:7">
@@ -27759,7 +27769,7 @@
         <v>661</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>126</v>

</xml_diff>